<commit_message>
Re-knit webpage and do some cleanup
</commit_message>
<xml_diff>
--- a/docs/data/output/survey_processing/eda_scheme6.xlsx
+++ b/docs/data/output/survey_processing/eda_scheme6.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TRM\trm_project\repo_trmg2\docs\data\output\survey_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{81E2E2AD-6802-432E-A8DA-59DA65FF5CEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C079BD-BC2D-42AD-887F-EE5FB721F64D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eda_scheme6" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
   <si>
     <t>tour_type</t>
   </si>
@@ -167,15 +167,12 @@
   </si>
   <si>
     <t>K12-O/OME</t>
-  </si>
-  <si>
-    <t>O-O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1292,11 +1289,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1314,10 +1311,10 @@
       <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="11" t="s">
@@ -1418,10 +1415,10 @@
       <c r="D2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>274</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>49624</v>
       </c>
       <c r="G2" s="1">
@@ -1514,10 +1511,10 @@
       <c r="D3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1979</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>358098</v>
       </c>
       <c r="G3" s="6">
@@ -1616,10 +1613,10 @@
       <c r="D4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="18">
         <v>3566</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <v>641617</v>
       </c>
       <c r="G4" s="17">
@@ -1718,10 +1715,10 @@
       <c r="D5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="22">
         <v>290</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>66697</v>
       </c>
       <c r="G5" s="21">
@@ -1818,10 +1815,10 @@
       <c r="D6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>777</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>249051</v>
       </c>
       <c r="G6" s="6">
@@ -1920,10 +1917,10 @@
       <c r="D7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="18">
         <v>2456</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="18">
         <v>701293</v>
       </c>
       <c r="G7" s="17">
@@ -2024,10 +2021,10 @@
       <c r="D8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="22">
         <v>1555</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>532573</v>
       </c>
       <c r="G8" s="21">
@@ -2128,10 +2125,10 @@
       <c r="D9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>3887</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>977872</v>
       </c>
       <c r="G9" s="6">
@@ -2232,10 +2229,10 @@
       <c r="D10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>2734</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <v>870710</v>
       </c>
       <c r="G10" s="6">
@@ -2336,10 +2333,10 @@
       <c r="D11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>4038</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>1131338</v>
       </c>
       <c r="G11" s="6">
@@ -2426,208 +2423,208 @@
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="18">
         <v>541</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="18">
         <v>122498</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="17">
         <v>-5.3999999999999999E-2</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="18">
         <v>-6.6000000000000003E-2</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="18">
         <v>-0.111</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="18">
         <v>0.105</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="18">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="18">
         <v>-5.0999999999999997E-2</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="18">
         <v>-4.5999999999999999E-2</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="18">
         <v>-2.3E-2</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="19">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="17">
         <v>42.8</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="18">
         <v>47.5</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="18">
         <v>6.6</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="18">
         <v>2.5</v>
       </c>
-      <c r="T12" s="25"/>
-      <c r="U12" s="5">
+      <c r="T12" s="26"/>
+      <c r="U12" s="18">
         <v>0.4</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="18">
         <v>0</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="19">
         <v>0.2</v>
       </c>
-      <c r="X12" s="6">
+      <c r="X12" s="17">
         <v>15.2</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y12" s="18">
         <v>57.4</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12" s="18">
         <v>7.7</v>
       </c>
-      <c r="AA12" s="7">
+      <c r="AA12" s="19">
         <v>19.600000000000001</v>
       </c>
-      <c r="AB12" s="15">
+      <c r="AB12" s="20">
         <v>9.18</v>
       </c>
-      <c r="AC12" s="6">
+      <c r="AC12" s="17">
         <v>0.34499999999999997</v>
       </c>
-      <c r="AD12" s="5">
+      <c r="AD12" s="18">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="AE12" s="5">
+      <c r="AE12" s="18">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="AF12" s="5">
+      <c r="AF12" s="18">
         <v>7.8E-2</v>
       </c>
-      <c r="AG12" s="5">
+      <c r="AG12" s="18">
         <v>0.122</v>
       </c>
-      <c r="AH12" s="7">
+      <c r="AH12" s="19">
         <v>0.36</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="5">
         <v>453</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="5">
         <v>120022</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="6">
         <v>0.17399999999999999</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="5">
         <v>-0.17</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="5">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="5">
         <v>-8.5000000000000006E-2</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="5">
         <v>-5.7000000000000002E-2</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="5">
         <v>0.34</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="5">
         <v>0.109</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="5">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13" s="7">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P13" s="17">
+      <c r="P13" s="6">
         <v>6.6</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="Q13" s="5">
         <v>39.6</v>
       </c>
-      <c r="R13" s="18">
+      <c r="R13" s="5">
         <v>10.5</v>
       </c>
-      <c r="S13" s="18">
+      <c r="S13" s="5">
         <v>0.6</v>
       </c>
-      <c r="T13" s="26">
+      <c r="T13" s="25">
         <v>33.4</v>
       </c>
-      <c r="U13" s="18">
+      <c r="U13" s="5">
         <v>6.9</v>
       </c>
-      <c r="V13" s="18">
+      <c r="V13" s="5">
         <v>0.2</v>
       </c>
-      <c r="W13" s="19">
+      <c r="W13" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="X13" s="17">
+      <c r="X13" s="6">
         <v>26.7</v>
       </c>
-      <c r="Y13" s="18">
+      <c r="Y13" s="5">
         <v>22.5</v>
       </c>
-      <c r="Z13" s="18">
+      <c r="Z13" s="5">
         <v>10</v>
       </c>
-      <c r="AA13" s="19">
+      <c r="AA13" s="7">
         <v>40.9</v>
       </c>
-      <c r="AB13" s="20">
+      <c r="AB13" s="15">
         <v>5.17</v>
       </c>
-      <c r="AC13" s="17">
+      <c r="AC13" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AD13" s="18">
+      <c r="AD13" s="5">
         <v>-0.05</v>
       </c>
-      <c r="AE13" s="18">
+      <c r="AE13" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AF13" s="18">
+      <c r="AF13" s="5">
         <v>0.108</v>
       </c>
-      <c r="AG13" s="18">
+      <c r="AG13" s="5">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="AH13" s="19">
+      <c r="AH13" s="7">
         <v>-3.2000000000000001E-2</v>
       </c>
     </row>
@@ -2639,15 +2636,15 @@
         <v>40</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>1621</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>490206</v>
       </c>
       <c r="G14" s="6">
@@ -2748,10 +2745,10 @@
       <c r="D15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="9">
         <v>3178</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>1116203</v>
       </c>
       <c r="G15" s="8">

</xml_diff>

<commit_message>
Correct detection of school pick up
Picking up at school (PUS) is now correct detected. This impacted
the EDA tables, which have been recreated. Now the EK12 trips
have a more reasonable distribution with 25% in the PM and 50%
in the AM.
</commit_message>
<xml_diff>
--- a/docs/data/output/survey_processing/eda_scheme6.xlsx
+++ b/docs/data/output/survey_processing/eda_scheme6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TRM\trm_project\repo_trmg2\docs\data\output\survey_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E84DE3-ACB4-403B-8E1B-26557C7A012A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EE2B1B-DE3B-4850-9B5A-0CCA31C811E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>tour_type</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>OMED</t>
-  </si>
-  <si>
-    <t>K12-O/OME</t>
   </si>
   <si>
     <t>EK12</t>
@@ -1408,92 +1405,96 @@
         <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="2">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="F2" s="2">
-        <v>48748</v>
+        <v>72087</v>
       </c>
       <c r="G2" s="1">
-        <v>0.108</v>
+        <v>0.107</v>
       </c>
       <c r="H2" s="2">
-        <v>0.14599999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="I2" s="2">
-        <v>9.4E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="J2" s="2">
-        <v>-7.0999999999999994E-2</v>
+        <v>-7.2999999999999995E-2</v>
       </c>
       <c r="K2" s="2">
-        <v>-5.7000000000000002E-2</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="L2" s="2">
-        <v>-7.2999999999999995E-2</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="M2" s="2">
-        <v>0.185</v>
+        <v>0.182</v>
       </c>
       <c r="N2" s="2">
-        <v>7.8E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="O2" s="3">
-        <v>1.7000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="P2" s="6">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Q2" s="5">
-        <v>97.6</v>
+        <v>97.8</v>
       </c>
       <c r="R2" s="25"/>
       <c r="S2" s="5">
         <v>0</v>
       </c>
       <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
+      <c r="U2" s="25">
+        <v>0.4</v>
+      </c>
       <c r="V2" s="5">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="W2" s="7">
         <v>0</v>
       </c>
       <c r="X2" s="1">
-        <v>78.599999999999994</v>
+        <v>53.1</v>
       </c>
       <c r="Y2" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="Z2" s="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>26.9</v>
+      </c>
       <c r="AA2" s="3">
-        <v>18.600000000000001</v>
+        <v>15.6</v>
       </c>
       <c r="AB2" s="4">
-        <v>5.38</v>
+        <v>5.39</v>
       </c>
       <c r="AC2" s="1">
-        <v>-0.04</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="AD2" s="2">
-        <v>-5.3999999999999999E-2</v>
+        <v>-3.6999999999999998E-2</v>
       </c>
       <c r="AE2" s="2">
-        <v>8.9999999999999993E-3</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AF2" s="2">
-        <v>-7.0000000000000001E-3</v>
+        <v>3.1E-2</v>
       </c>
       <c r="AG2" s="2">
-        <v>-0.11899999999999999</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="AH2" s="3">
-        <v>-3.4000000000000002E-2</v>
+        <v>-3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.45">
@@ -1510,92 +1511,92 @@
         <v>36</v>
       </c>
       <c r="E3" s="5">
-        <v>1982</v>
+        <v>1873</v>
       </c>
       <c r="F3" s="5">
-        <v>358975</v>
+        <v>339400</v>
       </c>
       <c r="G3" s="6">
-        <v>-6.6000000000000003E-2</v>
+        <v>-8.5000000000000006E-2</v>
       </c>
       <c r="H3" s="5">
-        <v>0.39400000000000002</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="I3" s="5">
-        <v>0.19800000000000001</v>
+        <v>0.185</v>
       </c>
       <c r="J3" s="5">
-        <v>-0.14899999999999999</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="K3" s="5">
-        <v>-0.108</v>
+        <v>-0.10100000000000001</v>
       </c>
       <c r="L3" s="5">
-        <v>-0.19700000000000001</v>
+        <v>-0.19</v>
       </c>
       <c r="M3" s="5">
-        <v>2.9000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="N3" s="5">
-        <v>5.3999999999999999E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="O3" s="7">
-        <v>-1.2E-2</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="P3" s="6">
-        <v>64.5</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="Q3" s="5">
-        <v>31</v>
+        <v>26.6</v>
       </c>
       <c r="R3" s="5">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="S3" s="5">
         <v>0.8</v>
       </c>
       <c r="T3" s="25"/>
       <c r="U3" s="5">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="V3" s="5">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="W3" s="7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="X3" s="6">
-        <v>14.2</v>
+        <v>15.4</v>
       </c>
       <c r="Y3" s="5">
-        <v>12.2</v>
+        <v>12.8</v>
       </c>
       <c r="Z3" s="5">
-        <v>31.5</v>
+        <v>27.9</v>
       </c>
       <c r="AA3" s="7">
-        <v>42</v>
+        <v>43.9</v>
       </c>
       <c r="AB3" s="15">
-        <v>5.56</v>
+        <v>5.47</v>
       </c>
       <c r="AC3" s="6">
-        <v>0.253</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="AD3" s="5">
-        <v>0.47699999999999998</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="AE3" s="5">
-        <v>9.1999999999999998E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="AF3" s="5">
-        <v>3.5000000000000003E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AG3" s="5">
-        <v>0.16700000000000001</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="AH3" s="7">
-        <v>0.114</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.45">
@@ -1615,10 +1616,10 @@
         <v>3566</v>
       </c>
       <c r="F4" s="18">
-        <v>641617</v>
+        <v>639632</v>
       </c>
       <c r="G4" s="17">
-        <v>-0.11899999999999999</v>
+        <v>-0.12</v>
       </c>
       <c r="H4" s="18">
         <v>0.55600000000000005</v>
@@ -1627,38 +1628,38 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="J4" s="18">
-        <v>-0.21099999999999999</v>
+        <v>-0.21</v>
       </c>
       <c r="K4" s="18">
-        <v>-0.14099999999999999</v>
+        <v>-0.14199999999999999</v>
       </c>
       <c r="L4" s="18">
         <v>-0.27600000000000002</v>
       </c>
       <c r="M4" s="18">
-        <v>-4.5999999999999999E-2</v>
+        <v>-4.8000000000000001E-2</v>
       </c>
       <c r="N4" s="18">
-        <v>4.5999999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="O4" s="19">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="P4" s="17">
-        <v>86.4</v>
+        <v>86.2</v>
       </c>
       <c r="Q4" s="18">
-        <v>6.7</v>
+        <v>7.9</v>
       </c>
       <c r="R4" s="18">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="S4" s="18">
         <v>2.1</v>
       </c>
       <c r="T4" s="26"/>
       <c r="U4" s="18">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V4" s="18">
         <v>1.2</v>
@@ -1667,34 +1668,34 @@
         <v>0.1</v>
       </c>
       <c r="X4" s="17">
-        <v>28.9</v>
+        <v>28.8</v>
       </c>
       <c r="Y4" s="18">
-        <v>17</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="Z4" s="18">
-        <v>27</v>
+        <v>27.1</v>
       </c>
       <c r="AA4" s="19">
-        <v>27.1</v>
+        <v>27.2</v>
       </c>
       <c r="AB4" s="20">
-        <v>10.75</v>
+        <v>10.72</v>
       </c>
       <c r="AC4" s="17">
-        <v>0.58799999999999997</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="AD4" s="18">
-        <v>0.156</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="AE4" s="18">
         <v>0.18099999999999999</v>
       </c>
       <c r="AF4" s="18">
-        <v>0.45300000000000001</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="AG4" s="18">
-        <v>0.159</v>
+        <v>0.16</v>
       </c>
       <c r="AH4" s="19">
         <v>0.39700000000000002</v>
@@ -1705,99 +1706,99 @@
         <v>38</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="22">
-        <v>287</v>
+        <v>357</v>
       </c>
       <c r="F5" s="22">
-        <v>65451</v>
+        <v>111814</v>
       </c>
       <c r="G5" s="21">
-        <v>0.104</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="H5" s="22">
-        <v>0.13700000000000001</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="I5" s="22">
-        <v>8.7999999999999995E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="J5" s="22">
-        <v>-6.7000000000000004E-2</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K5" s="22">
-        <v>-5.1999999999999998E-2</v>
+        <v>-5.3999999999999999E-2</v>
       </c>
       <c r="L5" s="22">
-        <v>-6.8000000000000005E-2</v>
+        <v>-7.1999999999999995E-2</v>
       </c>
       <c r="M5" s="22">
-        <v>0.17899999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="N5" s="22">
-        <v>7.2999999999999995E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="O5" s="23">
-        <v>1.9E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="P5" s="21">
-        <v>69.3</v>
+        <v>63.8</v>
       </c>
       <c r="Q5" s="22">
-        <v>29</v>
+        <v>34.6</v>
       </c>
       <c r="R5" s="22"/>
       <c r="S5" s="22">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="T5" s="25"/>
       <c r="U5" s="22">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V5" s="22">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="W5" s="23">
         <v>0</v>
       </c>
       <c r="X5" s="21">
-        <v>86.2</v>
+        <v>50.7</v>
       </c>
       <c r="Y5" s="22">
-        <v>7.4</v>
+        <v>12.1</v>
       </c>
       <c r="Z5" s="22">
-        <v>0.1</v>
+        <v>31.4</v>
       </c>
       <c r="AA5" s="23">
-        <v>6.3</v>
+        <v>5.8</v>
       </c>
       <c r="AB5" s="24">
-        <v>7.86</v>
+        <v>7.41</v>
       </c>
       <c r="AC5" s="21">
-        <v>0.159</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="AD5" s="22">
-        <v>0.186</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="AE5" s="22">
-        <v>-1.7000000000000001E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AF5" s="22">
-        <v>6.9000000000000006E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="AG5" s="22">
-        <v>8.3000000000000004E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="AH5" s="23">
-        <v>0.11799999999999999</v>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.45">
@@ -1805,7 +1806,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>37</v>
@@ -1814,92 +1815,92 @@
         <v>36</v>
       </c>
       <c r="E6" s="5">
-        <v>778</v>
+        <v>743</v>
       </c>
       <c r="F6" s="5">
-        <v>249420</v>
+        <v>234448</v>
       </c>
       <c r="G6" s="6">
-        <v>-5.2999999999999999E-2</v>
+        <v>-6.6000000000000003E-2</v>
       </c>
       <c r="H6" s="5">
-        <v>0.20599999999999999</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="I6" s="5">
-        <v>9.8000000000000004E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="J6" s="5">
-        <v>-7.3999999999999996E-2</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K6" s="5">
-        <v>-6.3E-2</v>
+        <v>-5.8000000000000003E-2</v>
       </c>
       <c r="L6" s="5">
-        <v>-0.10299999999999999</v>
+        <v>-0.1</v>
       </c>
       <c r="M6" s="5">
-        <v>2E-3</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
       <c r="N6" s="5">
-        <v>8.0000000000000002E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="O6" s="7">
-        <v>-2.4E-2</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="P6" s="6">
-        <v>54.7</v>
+        <v>57.1</v>
       </c>
       <c r="Q6" s="5">
-        <v>30.9</v>
+        <v>28.7</v>
       </c>
       <c r="R6" s="5">
-        <v>1.9</v>
+        <v>0.1</v>
       </c>
       <c r="S6" s="5">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="T6" s="25"/>
       <c r="U6" s="5">
-        <v>10.1</v>
+        <v>11.3</v>
       </c>
       <c r="V6" s="5">
         <v>0.1</v>
       </c>
       <c r="W6" s="7">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="X6" s="6">
-        <v>7.6</v>
+        <v>8.5</v>
       </c>
       <c r="Y6" s="5">
-        <v>28.3</v>
+        <v>29</v>
       </c>
       <c r="Z6" s="5">
-        <v>36.9</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="AA6" s="7">
-        <v>27.2</v>
+        <v>28.8</v>
       </c>
       <c r="AB6" s="15">
-        <v>4.6900000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AC6" s="6">
-        <v>0.20699999999999999</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="AD6" s="5">
-        <v>0.42099999999999999</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="AE6" s="5">
-        <v>7.2999999999999995E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="AF6" s="5">
-        <v>1.2999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="AG6" s="5">
-        <v>0.104</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="AH6" s="7">
-        <v>0.08</v>
+        <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.45">
@@ -1907,7 +1908,7 @@
         <v>38</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>39</v>
@@ -1916,99 +1917,99 @@
         <v>36</v>
       </c>
       <c r="E7" s="18">
-        <v>2459</v>
+        <v>2363</v>
       </c>
       <c r="F7" s="18">
-        <v>702169</v>
+        <v>680198</v>
       </c>
       <c r="G7" s="17">
-        <v>-9.1999999999999998E-2</v>
+        <v>-0.10299999999999999</v>
       </c>
       <c r="H7" s="18">
-        <v>0.38400000000000001</v>
+        <v>0.376</v>
       </c>
       <c r="I7" s="18">
-        <v>0.17599999999999999</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="J7" s="18">
-        <v>-0.13900000000000001</v>
+        <v>-0.13300000000000001</v>
       </c>
       <c r="K7" s="18">
-        <v>-0.10100000000000001</v>
+        <v>-9.8000000000000004E-2</v>
       </c>
       <c r="L7" s="18">
-        <v>-0.192</v>
+        <v>-0.188</v>
       </c>
       <c r="M7" s="18">
-        <v>-3.0000000000000001E-3</v>
+        <v>-0.02</v>
       </c>
       <c r="N7" s="18">
-        <v>6.3E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="O7" s="19">
-        <v>-0.01</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
       <c r="P7" s="17">
-        <v>68</v>
+        <v>67.5</v>
       </c>
       <c r="Q7" s="18">
-        <v>11.5</v>
+        <v>14</v>
       </c>
       <c r="R7" s="18">
-        <v>3.8</v>
+        <v>0.9</v>
       </c>
       <c r="S7" s="18">
         <v>1.6</v>
       </c>
       <c r="T7" s="18">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="U7" s="18">
-        <v>14.5</v>
+        <v>15.1</v>
       </c>
       <c r="V7" s="18">
         <v>0.3</v>
       </c>
       <c r="W7" s="19">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="X7" s="17">
-        <v>10.8</v>
+        <v>11.4</v>
       </c>
       <c r="Y7" s="18">
-        <v>49.2</v>
+        <v>50.4</v>
       </c>
       <c r="Z7" s="18">
-        <v>30.4</v>
+        <v>28.4</v>
       </c>
       <c r="AA7" s="19">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AB7" s="20">
-        <v>6.05</v>
+        <v>6.03</v>
       </c>
       <c r="AC7" s="17">
         <v>0.59399999999999997</v>
       </c>
       <c r="AD7" s="18">
-        <v>0.38600000000000001</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="AE7" s="18">
-        <v>0.13100000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="AF7" s="18">
-        <v>0.35299999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="AG7" s="18">
-        <v>0.29899999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="AH7" s="19">
-        <v>0.40200000000000002</v>
+        <v>0.40400000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>34</v>
@@ -2020,52 +2021,52 @@
         <v>36</v>
       </c>
       <c r="E8" s="22">
-        <v>1555</v>
+        <v>1689</v>
       </c>
       <c r="F8" s="22">
-        <v>532573</v>
+        <v>624708</v>
       </c>
       <c r="G8" s="21">
         <v>0.34</v>
       </c>
       <c r="H8" s="22">
-        <v>-0.24099999999999999</v>
+        <v>-0.20300000000000001</v>
       </c>
       <c r="I8" s="22">
-        <v>0.14799999999999999</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="J8" s="22">
-        <v>-0.16600000000000001</v>
+        <v>-0.16500000000000001</v>
       </c>
       <c r="K8" s="22">
-        <v>-0.11</v>
+        <v>-0.112</v>
       </c>
       <c r="L8" s="22">
-        <v>0.48899999999999999</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="M8" s="22">
-        <v>0.26</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="N8" s="22">
-        <v>0.124</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="O8" s="23">
-        <v>7.0999999999999994E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="P8" s="21">
-        <v>14.3</v>
+        <v>17.3</v>
       </c>
       <c r="Q8" s="22">
-        <v>51.6</v>
+        <v>57.7</v>
       </c>
       <c r="R8" s="22">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="S8" s="22">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="T8" s="5">
-        <v>25.1</v>
+        <v>21</v>
       </c>
       <c r="U8" s="22">
         <v>2.7</v>
@@ -2074,45 +2075,45 @@
         <v>0.4</v>
       </c>
       <c r="W8" s="23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="X8" s="21">
-        <v>46.3</v>
+        <v>39.5</v>
       </c>
       <c r="Y8" s="22">
-        <v>15.9</v>
+        <v>17.5</v>
       </c>
       <c r="Z8" s="22">
-        <v>22.4</v>
+        <v>28.5</v>
       </c>
       <c r="AA8" s="23">
-        <v>15.4</v>
+        <v>14.5</v>
       </c>
       <c r="AB8" s="24">
-        <v>4.8600000000000003</v>
+        <v>4.92</v>
       </c>
       <c r="AC8" s="21">
-        <v>-5.3999999999999999E-2</v>
+        <v>-5.1999999999999998E-2</v>
       </c>
       <c r="AD8" s="22">
-        <v>-0.10199999999999999</v>
+        <v>-0.108</v>
       </c>
       <c r="AE8" s="22">
-        <v>-4.9000000000000002E-2</v>
+        <v>-4.2999999999999997E-2</v>
       </c>
       <c r="AF8" s="22">
-        <v>6.7000000000000004E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="AG8" s="22">
-        <v>-7.3999999999999996E-2</v>
+        <v>-0.08</v>
       </c>
       <c r="AH8" s="23">
-        <v>-0.10199999999999999</v>
+        <v>-9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>34</v>
@@ -2124,46 +2125,46 @@
         <v>41</v>
       </c>
       <c r="E9" s="5">
-        <v>3887</v>
+        <v>3900</v>
       </c>
       <c r="F9" s="5">
-        <v>977872</v>
+        <v>981669</v>
       </c>
       <c r="G9" s="6">
-        <v>-2E-3</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="H9" s="5">
-        <v>-0.125</v>
+        <v>-0.126</v>
       </c>
       <c r="I9" s="5">
         <v>-7.3999999999999996E-2</v>
       </c>
       <c r="J9" s="5">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="K9" s="5">
         <v>-1E-3</v>
       </c>
       <c r="L9" s="5">
-        <v>0.02</v>
+        <v>1.9E-2</v>
       </c>
       <c r="M9" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="N9" s="5">
-        <v>-8.9999999999999993E-3</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="O9" s="7">
-        <v>-2.5000000000000001E-2</v>
+        <v>-2.7E-2</v>
       </c>
       <c r="P9" s="6">
-        <v>39.299999999999997</v>
+        <v>38.9</v>
       </c>
       <c r="Q9" s="5">
-        <v>45.9</v>
+        <v>49.3</v>
       </c>
       <c r="R9" s="5">
-        <v>4.5999999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="S9" s="5">
         <v>1.5</v>
@@ -2172,51 +2173,51 @@
         <v>0.5</v>
       </c>
       <c r="U9" s="5">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
       <c r="V9" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="W9" s="7">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="X9" s="6">
-        <v>10.4</v>
+        <v>10.5</v>
       </c>
       <c r="Y9" s="5">
-        <v>27.5</v>
+        <v>27.1</v>
       </c>
       <c r="Z9" s="5">
-        <v>23.7</v>
+        <v>23.6</v>
       </c>
       <c r="AA9" s="7">
-        <v>38.5</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="AB9" s="15">
-        <v>6.74</v>
+        <v>6.66</v>
       </c>
       <c r="AC9" s="6">
-        <v>0.218</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="AD9" s="5">
-        <v>0.11</v>
+        <v>0.105</v>
       </c>
       <c r="AE9" s="5">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AF9" s="5">
-        <v>0.111</v>
+        <v>0.108</v>
       </c>
       <c r="AG9" s="5">
-        <v>0.371</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="AH9" s="7">
-        <v>0.13800000000000001</v>
+        <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>34</v>
@@ -2228,99 +2229,99 @@
         <v>42</v>
       </c>
       <c r="E10" s="5">
-        <v>2734</v>
+        <v>2592</v>
       </c>
       <c r="F10" s="5">
-        <v>870710</v>
+        <v>818413</v>
       </c>
       <c r="G10" s="6">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>-6.5000000000000002E-2</v>
+      </c>
+      <c r="J10" s="5">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="K10" s="5">
         <v>2.4E-2</v>
       </c>
-      <c r="H10" s="5">
-        <v>-3.4000000000000002E-2</v>
-      </c>
-      <c r="I10" s="5">
-        <v>-4.2000000000000003E-2</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="K10" s="5">
-        <v>7.0000000000000001E-3</v>
-      </c>
       <c r="L10" s="5">
-        <v>-5.7000000000000002E-2</v>
+        <v>-6.2E-2</v>
       </c>
       <c r="M10" s="5">
-        <v>7.5999999999999998E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="N10" s="5">
-        <v>3.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="O10" s="7">
-        <v>-8.0000000000000002E-3</v>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="P10" s="6">
-        <v>25.4</v>
+        <v>23.3</v>
       </c>
       <c r="Q10" s="5">
-        <v>36</v>
+        <v>31.9</v>
       </c>
       <c r="R10" s="5">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="S10" s="5">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="T10" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="U10" s="5">
+        <v>41.2</v>
+      </c>
+      <c r="V10" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="W10" s="7">
         <v>0.3</v>
       </c>
-      <c r="U10" s="5">
-        <v>34.5</v>
-      </c>
-      <c r="V10" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="W10" s="7">
-        <v>0.2</v>
-      </c>
       <c r="X10" s="6">
-        <v>14</v>
+        <v>15.1</v>
       </c>
       <c r="Y10" s="5">
-        <v>25.6</v>
+        <v>25.1</v>
       </c>
       <c r="Z10" s="5">
-        <v>32.799999999999997</v>
+        <v>30.3</v>
       </c>
       <c r="AA10" s="7">
-        <v>27.6</v>
+        <v>29.5</v>
       </c>
       <c r="AB10" s="15">
-        <v>3.43</v>
+        <v>3.1</v>
       </c>
       <c r="AC10" s="6">
-        <v>6.5000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="AD10" s="5">
-        <v>4.5999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AE10" s="5">
-        <v>1.2999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AF10" s="5">
-        <v>4.7E-2</v>
+        <v>0.03</v>
       </c>
       <c r="AG10" s="5">
-        <v>0.16300000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="AH10" s="7">
-        <v>8.9999999999999993E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>34</v>
@@ -2332,10 +2333,10 @@
         <v>36</v>
       </c>
       <c r="E11" s="5">
-        <v>4038</v>
+        <v>4036</v>
       </c>
       <c r="F11" s="5">
-        <v>1131338</v>
+        <v>1130729</v>
       </c>
       <c r="G11" s="6">
         <v>-0.127</v>
@@ -2347,7 +2348,7 @@
         <v>-0.221</v>
       </c>
       <c r="J11" s="5">
-        <v>0.17599999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="K11" s="5">
         <v>0.13</v>
@@ -2356,7 +2357,7 @@
         <v>-0.152</v>
       </c>
       <c r="M11" s="5">
-        <v>-8.6999999999999994E-2</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
       <c r="N11" s="5">
         <v>-2.7E-2</v>
@@ -2365,64 +2366,64 @@
         <v>-1.7000000000000001E-2</v>
       </c>
       <c r="P11" s="6">
-        <v>43.7</v>
+        <v>43.5</v>
       </c>
       <c r="Q11" s="5">
-        <v>47.1</v>
+        <v>49.4</v>
       </c>
       <c r="R11" s="5">
-        <v>3.1</v>
+        <v>0.5</v>
       </c>
       <c r="S11" s="5">
         <v>0.7</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="5">
-        <v>4.9000000000000004</v>
+        <v>5.2</v>
       </c>
       <c r="V11" s="5">
         <v>0.5</v>
       </c>
       <c r="W11" s="7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="X11" s="6">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="Y11" s="5">
         <v>43.5</v>
       </c>
       <c r="Z11" s="5">
-        <v>24.5</v>
+        <v>24.3</v>
       </c>
       <c r="AA11" s="7">
-        <v>28.3</v>
+        <v>28.4</v>
       </c>
       <c r="AB11" s="15">
-        <v>4.55</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="AC11" s="6">
-        <v>0.308</v>
+        <v>0.311</v>
       </c>
       <c r="AD11" s="5">
-        <v>0.70599999999999996</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="AE11" s="5">
-        <v>-7.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="AF11" s="5">
-        <v>1.2999999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AG11" s="5">
-        <v>8.4000000000000005E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="AH11" s="7">
-        <v>0.106</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>34</v>
@@ -2434,28 +2435,28 @@
         <v>36</v>
       </c>
       <c r="E12" s="18">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F12" s="18">
-        <v>122498</v>
+        <v>123622</v>
       </c>
       <c r="G12" s="17">
-        <v>-5.3999999999999999E-2</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
       <c r="H12" s="18">
         <v>-6.6000000000000003E-2</v>
       </c>
       <c r="I12" s="18">
-        <v>-0.111</v>
+        <v>-0.113</v>
       </c>
       <c r="J12" s="18">
-        <v>0.105</v>
+        <v>0.106</v>
       </c>
       <c r="K12" s="18">
-        <v>7.4999999999999997E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="L12" s="18">
-        <v>-5.0999999999999997E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="M12" s="18">
         <v>-4.5999999999999999E-2</v>
@@ -2464,16 +2465,16 @@
         <v>-2.3E-2</v>
       </c>
       <c r="O12" s="19">
-        <v>-8.0000000000000002E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="P12" s="17">
-        <v>42.8</v>
+        <v>41.1</v>
       </c>
       <c r="Q12" s="18">
-        <v>47.5</v>
+        <v>48.3</v>
       </c>
       <c r="R12" s="18">
-        <v>6.6</v>
+        <v>1.7</v>
       </c>
       <c r="S12" s="18">
         <v>2.5</v>
@@ -2486,138 +2487,138 @@
         <v>0</v>
       </c>
       <c r="W12" s="19">
-        <v>0.2</v>
+        <v>5.9</v>
       </c>
       <c r="X12" s="17">
-        <v>15.2</v>
+        <v>15.4</v>
       </c>
       <c r="Y12" s="18">
-        <v>57.4</v>
+        <v>57.7</v>
       </c>
       <c r="Z12" s="18">
-        <v>19.600000000000001</v>
+        <v>19.2</v>
       </c>
       <c r="AA12" s="19">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
       <c r="AB12" s="20">
-        <v>9.18</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="AC12" s="17">
-        <v>0.34499999999999997</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="AD12" s="18">
-        <v>6.0999999999999999E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="AE12" s="18">
-        <v>-4.4999999999999998E-2</v>
+        <v>-4.5999999999999999E-2</v>
       </c>
       <c r="AF12" s="18">
-        <v>7.8E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="AG12" s="18">
-        <v>0.122</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="AH12" s="19">
-        <v>0.36</v>
+        <v>0.41199999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="5">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="F13" s="5">
-        <v>120022</v>
+        <v>124235</v>
       </c>
       <c r="G13" s="6">
-        <v>0.17399999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H13" s="5">
-        <v>-0.17</v>
+        <v>-0.17299999999999999</v>
       </c>
       <c r="I13" s="5">
-        <v>7.9000000000000001E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="J13" s="5">
-        <v>-8.5000000000000006E-2</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
       <c r="K13" s="5">
-        <v>-5.7000000000000002E-2</v>
+        <v>-5.8999999999999997E-2</v>
       </c>
       <c r="L13" s="5">
-        <v>0.34</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="M13" s="5">
         <v>0.109</v>
       </c>
       <c r="N13" s="5">
-        <v>7.0999999999999994E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="O13" s="7">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="P13" s="6">
-        <v>6.6</v>
+        <v>6.3</v>
       </c>
       <c r="Q13" s="5">
-        <v>39.6</v>
+        <v>47</v>
       </c>
       <c r="R13" s="5">
-        <v>10.5</v>
+        <v>0.3</v>
       </c>
       <c r="S13" s="5">
         <v>0.6</v>
       </c>
       <c r="T13" s="25">
-        <v>33.4</v>
+        <v>34.5</v>
       </c>
       <c r="U13" s="5">
-        <v>6.9</v>
+        <v>6.7</v>
       </c>
       <c r="V13" s="5">
         <v>0.2</v>
       </c>
       <c r="W13" s="7">
-        <v>2.2000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="X13" s="6">
-        <v>26.7</v>
+        <v>27.6</v>
       </c>
       <c r="Y13" s="5">
-        <v>22.5</v>
+        <v>22.1</v>
       </c>
       <c r="Z13" s="5">
-        <v>40.9</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="AA13" s="7">
-        <v>10</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="AB13" s="15">
-        <v>5.17</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="AC13" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="AD13" s="5">
-        <v>-0.05</v>
+        <v>-5.1999999999999998E-2</v>
       </c>
       <c r="AE13" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AF13" s="5">
-        <v>0.108</v>
+        <v>0.107</v>
       </c>
       <c r="AG13" s="5">
         <v>8.9999999999999993E-3</v>
@@ -2628,10 +2629,10 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>37</v>
@@ -2640,102 +2641,102 @@
         <v>36</v>
       </c>
       <c r="E14" s="5">
-        <v>1621</v>
+        <v>1657</v>
       </c>
       <c r="F14" s="5">
-        <v>490206</v>
+        <v>510938</v>
       </c>
       <c r="G14" s="6">
-        <v>-5.0000000000000001E-3</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="H14" s="5">
-        <v>-2.9000000000000001E-2</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="I14" s="5">
-        <v>-3.9E-2</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="J14" s="5">
-        <v>1E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="K14" s="5">
-        <v>-3.0000000000000001E-3</v>
+        <v>-2E-3</v>
       </c>
       <c r="L14" s="5">
-        <v>-2.9000000000000001E-2</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="M14" s="5">
-        <v>0.03</v>
+        <v>2.7E-2</v>
       </c>
       <c r="N14" s="5">
-        <v>-1.2999999999999999E-2</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="O14" s="7">
-        <v>-2.5999999999999999E-2</v>
+        <v>-2.8000000000000001E-2</v>
       </c>
       <c r="P14" s="6">
-        <v>23.3</v>
+        <v>23.6</v>
       </c>
       <c r="Q14" s="5">
-        <v>45.4</v>
+        <v>49.1</v>
       </c>
       <c r="R14" s="5">
-        <v>6.2</v>
+        <v>1.2</v>
       </c>
       <c r="S14" s="5">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="T14" s="5">
         <v>0.9</v>
       </c>
       <c r="U14" s="5">
-        <v>14.3</v>
+        <v>15</v>
       </c>
       <c r="V14" s="5">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="W14" s="7">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="X14" s="6">
-        <v>13.6</v>
+        <v>13.1</v>
       </c>
       <c r="Y14" s="5">
-        <v>41.6</v>
+        <v>41.5</v>
       </c>
       <c r="Z14" s="5">
-        <v>27.4</v>
+        <v>27.3</v>
       </c>
       <c r="AA14" s="7">
-        <v>17.399999999999999</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="AB14" s="15">
-        <v>5.05</v>
+        <v>4.95</v>
       </c>
       <c r="AC14" s="6">
-        <v>0.27100000000000002</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="AD14" s="5">
-        <v>5.8999999999999997E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="AE14" s="5">
-        <v>9.2999999999999999E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="AF14" s="5">
-        <v>0.14399999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="AG14" s="5">
-        <v>0.35699999999999998</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="AH14" s="7">
-        <v>0.20599999999999999</v>
+        <v>0.19900000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>43</v>
@@ -2744,53 +2745,53 @@
         <v>36</v>
       </c>
       <c r="E15" s="9">
-        <v>3178</v>
+        <v>3194</v>
       </c>
       <c r="F15" s="9">
-        <v>1116203</v>
+        <v>1128123</v>
       </c>
       <c r="G15" s="8">
-        <v>-8.5999999999999993E-2</v>
+        <v>-8.6999999999999994E-2</v>
       </c>
       <c r="H15" s="9">
-        <v>-0.13200000000000001</v>
+        <v>-0.13400000000000001</v>
       </c>
       <c r="I15" s="9">
-        <v>-0.19600000000000001</v>
+        <v>-0.19800000000000001</v>
       </c>
       <c r="J15" s="9">
-        <v>0.14199999999999999</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="K15" s="9">
-        <v>8.3000000000000004E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="L15" s="9">
-        <v>-0.107</v>
+        <v>-0.108</v>
       </c>
       <c r="M15" s="9">
-        <v>-3.3000000000000002E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="N15" s="9">
         <v>-6.2E-2</v>
       </c>
       <c r="O15" s="10">
-        <v>-4.1000000000000002E-2</v>
+        <v>-4.2000000000000003E-2</v>
       </c>
       <c r="P15" s="8">
-        <v>40.9</v>
+        <v>41.1</v>
       </c>
       <c r="Q15" s="9">
-        <v>46.5</v>
+        <v>51.3</v>
       </c>
       <c r="R15" s="9">
-        <v>5.6</v>
+        <v>0.5</v>
       </c>
       <c r="S15" s="9">
         <v>0.7</v>
       </c>
       <c r="T15" s="9"/>
       <c r="U15" s="9">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="V15" s="9">
         <v>0.4</v>
@@ -2799,37 +2800,37 @@
         <v>0.2</v>
       </c>
       <c r="X15" s="8">
-        <v>5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Y15" s="9">
-        <v>55</v>
+        <v>54.9</v>
       </c>
       <c r="Z15" s="9">
-        <v>22.1</v>
+        <v>22.3</v>
       </c>
       <c r="AA15" s="10">
-        <v>18</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="AB15" s="16">
         <v>4.58</v>
       </c>
       <c r="AC15" s="8">
-        <v>0.29199999999999998</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="AD15" s="9">
-        <v>0.67800000000000005</v>
+        <v>0.68</v>
       </c>
       <c r="AE15" s="9">
-        <v>3.4000000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AF15" s="9">
-        <v>1.4999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AG15" s="9">
-        <v>0.1</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="AH15" s="10">
-        <v>0.106</v>
+        <v>0.108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update tod def in survey processing
</commit_message>
<xml_diff>
--- a/docs/data/output/survey_processing/eda_scheme6.xlsx
+++ b/docs/data/output/survey_processing/eda_scheme6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TRM\trm_project\repo_trmg2\docs\data\output\survey_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EE2B1B-DE3B-4850-9B5A-0CCA31C811E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68057A6-7129-4923-8C62-36295BD9BB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7298" yWindow="1920" windowWidth="17489" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eda_scheme6" sheetId="1" r:id="rId1"/>
@@ -1423,7 +1423,7 @@
         <v>0.15</v>
       </c>
       <c r="I2" s="2">
-        <v>0.10100000000000001</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="J2" s="2">
         <v>-7.2999999999999995E-2</v>
@@ -1467,13 +1467,13 @@
         <v>53.1</v>
       </c>
       <c r="Y2" s="2">
-        <v>4.4000000000000004</v>
+        <v>6.2</v>
       </c>
       <c r="Z2" s="2">
-        <v>26.9</v>
+        <v>26.4</v>
       </c>
       <c r="AA2" s="3">
-        <v>15.6</v>
+        <v>14.3</v>
       </c>
       <c r="AB2" s="4">
         <v>5.39</v>
@@ -1523,7 +1523,7 @@
         <v>0.38100000000000001</v>
       </c>
       <c r="I3" s="5">
-        <v>0.185</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="J3" s="5">
         <v>-0.14000000000000001</v>
@@ -1569,13 +1569,13 @@
         <v>15.4</v>
       </c>
       <c r="Y3" s="5">
-        <v>12.8</v>
+        <v>15.1</v>
       </c>
       <c r="Z3" s="5">
-        <v>27.9</v>
+        <v>30</v>
       </c>
       <c r="AA3" s="7">
-        <v>43.9</v>
+        <v>39.5</v>
       </c>
       <c r="AB3" s="15">
         <v>5.47</v>
@@ -1625,7 +1625,7 @@
         <v>0.55600000000000005</v>
       </c>
       <c r="I4" s="18">
-        <v>0.29699999999999999</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="J4" s="18">
         <v>-0.21</v>
@@ -1671,13 +1671,13 @@
         <v>28.8</v>
       </c>
       <c r="Y4" s="18">
-        <v>16.899999999999999</v>
+        <v>19.3</v>
       </c>
       <c r="Z4" s="18">
-        <v>27.1</v>
+        <v>28.2</v>
       </c>
       <c r="AA4" s="19">
-        <v>27.2</v>
+        <v>23.7</v>
       </c>
       <c r="AB4" s="20">
         <v>10.72</v>
@@ -1727,7 +1727,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="I5" s="22">
-        <v>9.9000000000000005E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="J5" s="22">
         <v>-7.0000000000000007E-2</v>
@@ -1771,13 +1771,13 @@
         <v>50.7</v>
       </c>
       <c r="Y5" s="22">
-        <v>12.1</v>
+        <v>14.2</v>
       </c>
       <c r="Z5" s="22">
-        <v>31.4</v>
+        <v>30.5</v>
       </c>
       <c r="AA5" s="23">
-        <v>5.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AB5" s="24">
         <v>7.41</v>
@@ -1827,7 +1827,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="I6" s="5">
-        <v>9.0999999999999998E-2</v>
+        <v>-3.7999999999999999E-2</v>
       </c>
       <c r="J6" s="5">
         <v>-7.0000000000000007E-2</v>
@@ -1873,13 +1873,13 @@
         <v>8.5</v>
       </c>
       <c r="Y6" s="5">
-        <v>29</v>
+        <v>31.5</v>
       </c>
       <c r="Z6" s="5">
-        <v>33.700000000000003</v>
+        <v>35</v>
       </c>
       <c r="AA6" s="7">
-        <v>28.8</v>
+        <v>25</v>
       </c>
       <c r="AB6" s="15">
         <v>4.5999999999999996</v>
@@ -1929,7 +1929,7 @@
         <v>0.376</v>
       </c>
       <c r="I7" s="18">
-        <v>0.16800000000000001</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="J7" s="18">
         <v>-0.13300000000000001</v>
@@ -1977,13 +1977,13 @@
         <v>11.4</v>
       </c>
       <c r="Y7" s="18">
-        <v>50.4</v>
+        <v>53.3</v>
       </c>
       <c r="Z7" s="18">
-        <v>28.4</v>
+        <v>27.5</v>
       </c>
       <c r="AA7" s="19">
-        <v>9.8000000000000007</v>
+        <v>7.8</v>
       </c>
       <c r="AB7" s="20">
         <v>6.03</v>
@@ -2033,7 +2033,7 @@
         <v>-0.20300000000000001</v>
       </c>
       <c r="I8" s="22">
-        <v>0.14099999999999999</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="J8" s="22">
         <v>-0.16500000000000001</v>
@@ -2081,13 +2081,13 @@
         <v>39.5</v>
       </c>
       <c r="Y8" s="22">
-        <v>17.5</v>
+        <v>25.1</v>
       </c>
       <c r="Z8" s="22">
-        <v>28.5</v>
+        <v>21.5</v>
       </c>
       <c r="AA8" s="23">
-        <v>14.5</v>
+        <v>14</v>
       </c>
       <c r="AB8" s="24">
         <v>4.92</v>
@@ -2137,7 +2137,7 @@
         <v>-0.126</v>
       </c>
       <c r="I9" s="5">
-        <v>-7.3999999999999996E-2</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="J9" s="5">
         <v>1.0999999999999999E-2</v>
@@ -2185,13 +2185,13 @@
         <v>10.5</v>
       </c>
       <c r="Y9" s="5">
-        <v>27.1</v>
+        <v>30.2</v>
       </c>
       <c r="Z9" s="5">
-        <v>23.6</v>
+        <v>24.7</v>
       </c>
       <c r="AA9" s="7">
-        <v>38.700000000000003</v>
+        <v>34.6</v>
       </c>
       <c r="AB9" s="15">
         <v>6.66</v>
@@ -2241,7 +2241,7 @@
         <v>-3.6999999999999998E-2</v>
       </c>
       <c r="I10" s="5">
-        <v>-6.5000000000000002E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="J10" s="5">
         <v>4.1000000000000002E-2</v>
@@ -2289,13 +2289,13 @@
         <v>15.1</v>
       </c>
       <c r="Y10" s="5">
-        <v>25.1</v>
+        <v>30.2</v>
       </c>
       <c r="Z10" s="5">
-        <v>30.3</v>
+        <v>27.9</v>
       </c>
       <c r="AA10" s="7">
-        <v>29.5</v>
+        <v>26.8</v>
       </c>
       <c r="AB10" s="15">
         <v>3.1</v>
@@ -2345,7 +2345,7 @@
         <v>-0.121</v>
       </c>
       <c r="I11" s="5">
-        <v>-0.221</v>
+        <v>-0.157</v>
       </c>
       <c r="J11" s="5">
         <v>0.17399999999999999</v>
@@ -2391,13 +2391,13 @@
         <v>3.8</v>
       </c>
       <c r="Y11" s="5">
-        <v>43.5</v>
+        <v>47.3</v>
       </c>
       <c r="Z11" s="5">
-        <v>24.3</v>
+        <v>22.9</v>
       </c>
       <c r="AA11" s="7">
-        <v>28.4</v>
+        <v>26</v>
       </c>
       <c r="AB11" s="15">
         <v>4.5199999999999996</v>
@@ -2447,7 +2447,7 @@
         <v>-6.6000000000000003E-2</v>
       </c>
       <c r="I12" s="18">
-        <v>-0.113</v>
+        <v>-6.9000000000000006E-2</v>
       </c>
       <c r="J12" s="18">
         <v>0.106</v>
@@ -2493,13 +2493,13 @@
         <v>15.4</v>
       </c>
       <c r="Y12" s="18">
-        <v>57.7</v>
+        <v>60.8</v>
       </c>
       <c r="Z12" s="18">
-        <v>19.2</v>
+        <v>17.3</v>
       </c>
       <c r="AA12" s="19">
-        <v>7.6</v>
+        <v>6.4</v>
       </c>
       <c r="AB12" s="20">
         <v>9.2799999999999994</v>
@@ -2549,7 +2549,7 @@
         <v>-0.17299999999999999</v>
       </c>
       <c r="I13" s="5">
-        <v>7.8E-2</v>
+        <v>0.189</v>
       </c>
       <c r="J13" s="5">
         <v>-8.5999999999999993E-2</v>
@@ -2597,13 +2597,13 @@
         <v>27.6</v>
       </c>
       <c r="Y13" s="5">
-        <v>22.1</v>
+        <v>34.9</v>
       </c>
       <c r="Z13" s="5">
-        <v>40.700000000000003</v>
+        <v>28.5</v>
       </c>
       <c r="AA13" s="7">
-        <v>9.6999999999999993</v>
+        <v>8.9</v>
       </c>
       <c r="AB13" s="15">
         <v>5.0999999999999996</v>
@@ -2653,7 +2653,7 @@
         <v>-3.3000000000000002E-2</v>
       </c>
       <c r="I14" s="5">
-        <v>-4.3999999999999997E-2</v>
+        <v>-0.04</v>
       </c>
       <c r="J14" s="5">
         <v>8.0000000000000002E-3</v>
@@ -2701,13 +2701,13 @@
         <v>13.1</v>
       </c>
       <c r="Y14" s="5">
-        <v>41.5</v>
+        <v>46</v>
       </c>
       <c r="Z14" s="5">
-        <v>27.3</v>
+        <v>24.6</v>
       </c>
       <c r="AA14" s="7">
-        <v>18.100000000000001</v>
+        <v>16.2</v>
       </c>
       <c r="AB14" s="15">
         <v>4.95</v>
@@ -2757,7 +2757,7 @@
         <v>-0.13400000000000001</v>
       </c>
       <c r="I15" s="9">
-        <v>-0.19800000000000001</v>
+        <v>-0.13</v>
       </c>
       <c r="J15" s="9">
         <v>0.14499999999999999</v>
@@ -2803,13 +2803,13 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="Y15" s="9">
-        <v>54.9</v>
+        <v>60.1</v>
       </c>
       <c r="Z15" s="9">
-        <v>22.3</v>
+        <v>18.8</v>
       </c>
       <c r="AA15" s="10">
-        <v>17.899999999999999</v>
+        <v>16.2</v>
       </c>
       <c r="AB15" s="16">
         <v>4.58</v>
@@ -2895,15 +2895,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC273F68D44EF549AD1BD0E5D55B5B7C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="315063b799ab555b4e77865ce3b3361e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="35b81125-b047-47c8-b0b0-722baac7a528" xmlns:ns3="5fe89d89-77ff-4a7d-998d-403e04f568fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cfebddd8dbdab9d9b5a54d21a7ba6ecf" ns2:_="" ns3:_="">
     <xsd:import namespace="35b81125-b047-47c8-b0b0-722baac7a528"/>
@@ -3108,6 +3099,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3115,14 +3115,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB894063-DC05-4856-80EA-85608E1C259A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC82E5DB-FE26-4367-9CC7-F53ADB13D439}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3141,6 +3133,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB894063-DC05-4856-80EA-85608E1C259A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A86CA0-EF49-4650-8CD5-71490CFDB9D6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Replace mode_simple2 field with mode_final
This also slightly changes the modes. HOV is split into HOV2 and HOV3+.
Walk and bike are combined into walkbike. Other RMDs will need to be
updated due to these changes.
</commit_message>
<xml_diff>
--- a/docs/data/output/survey_processing/eda_scheme6.xlsx
+++ b/docs/data/output/survey_processing/eda_scheme6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TRM\trm_project\repo_trmg2\docs\data\output\survey_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68057A6-7129-4923-8C62-36295BD9BB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE092756-534A-4618-8788-AEA9C7697229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7298" yWindow="1920" windowWidth="17489" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eda_scheme6" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>pct_sov</t>
   </si>
   <si>
-    <t>pct_hov</t>
-  </si>
-  <si>
     <t>pct_auto_pay</t>
   </si>
   <si>
@@ -82,12 +79,6 @@
     <t>pct_school_bus</t>
   </si>
   <si>
-    <t>pct_walk</t>
-  </si>
-  <si>
-    <t>pct_bike</t>
-  </si>
-  <si>
     <t>pct_other</t>
   </si>
   <si>
@@ -164,6 +155,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>pct_hov2</t>
+  </si>
+  <si>
+    <t>pct_hov3</t>
+  </si>
+  <si>
+    <t>pct_walkbike</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -1343,72 +1345,72 @@
         <v>15</v>
       </c>
       <c r="Q1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="V1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="X1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="Z1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="12" t="s">
+      <c r="AB1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AC1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AE1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AF1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AH1" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="AF1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2">
         <v>324</v>
@@ -1447,20 +1449,22 @@
         <v>1.5</v>
       </c>
       <c r="Q2" s="5">
-        <v>97.8</v>
-      </c>
-      <c r="R2" s="25"/>
+        <v>49.2</v>
+      </c>
+      <c r="R2" s="5">
+        <v>48.4</v>
+      </c>
       <c r="S2" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="T2" s="5"/>
+      <c r="U2" s="25">
         <v>0</v>
       </c>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25">
-        <v>0.4</v>
-      </c>
       <c r="V2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="W2" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="W2" s="25">
         <v>0</v>
       </c>
       <c r="X2" s="1">
@@ -1499,16 +1503,16 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="5">
         <v>1873</v>
@@ -1544,26 +1548,28 @@
         <v>-1.6E-2</v>
       </c>
       <c r="P3" s="6">
-        <v>68.099999999999994</v>
+        <v>67.2</v>
       </c>
       <c r="Q3" s="5">
-        <v>26.6</v>
+        <v>15.8</v>
       </c>
       <c r="R3" s="5">
+        <v>10.1</v>
+      </c>
+      <c r="S3" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="W3" s="25">
         <v>0.1</v>
-      </c>
-      <c r="S3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="T3" s="25"/>
-      <c r="U3" s="5">
-        <v>3.8</v>
-      </c>
-      <c r="V3" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="W3" s="7">
-        <v>0.2</v>
       </c>
       <c r="X3" s="6">
         <v>15.4</v>
@@ -1601,16 +1607,16 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="18">
         <v>3566</v>
@@ -1646,26 +1652,28 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="P4" s="17">
-        <v>86.2</v>
+        <v>85.3</v>
       </c>
       <c r="Q4" s="18">
-        <v>7.9</v>
+        <v>4.8</v>
       </c>
       <c r="R4" s="18">
-        <v>0.5</v>
+        <v>1.8</v>
       </c>
       <c r="S4" s="18">
+        <v>2.9</v>
+      </c>
+      <c r="T4" s="18">
         <v>2.1</v>
       </c>
-      <c r="T4" s="26"/>
       <c r="U4" s="18">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="V4" s="18">
-        <v>1.2</v>
-      </c>
-      <c r="W4" s="19">
-        <v>0.1</v>
+        <v>3.1</v>
+      </c>
+      <c r="W4" s="26">
+        <v>0</v>
       </c>
       <c r="X4" s="17">
         <v>28.8</v>
@@ -1703,16 +1711,16 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="22">
         <v>357</v>
@@ -1751,20 +1759,24 @@
         <v>63.8</v>
       </c>
       <c r="Q5" s="22">
-        <v>34.6</v>
-      </c>
-      <c r="R5" s="22"/>
+        <v>23.4</v>
+      </c>
+      <c r="R5" s="22">
+        <v>11.1</v>
+      </c>
       <c r="S5" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="T5" s="22">
         <v>0.3</v>
       </c>
-      <c r="T5" s="25"/>
       <c r="U5" s="22">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="V5" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="W5" s="23">
+        <v>1.3</v>
+      </c>
+      <c r="W5" s="25">
         <v>0</v>
       </c>
       <c r="X5" s="21">
@@ -1803,16 +1815,16 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="5">
         <v>743</v>
@@ -1848,26 +1860,28 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="P6" s="6">
-        <v>57.1</v>
+        <v>56.9</v>
       </c>
       <c r="Q6" s="5">
-        <v>28.7</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="R6" s="5">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="S6" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="T6" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="T6" s="25"/>
       <c r="U6" s="5">
-        <v>11.3</v>
+        <v>0</v>
       </c>
       <c r="V6" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="W6" s="7">
-        <v>0.4</v>
+        <v>11.5</v>
+      </c>
+      <c r="W6" s="25">
+        <v>0.2</v>
       </c>
       <c r="X6" s="6">
         <v>8.5</v>
@@ -1905,16 +1919,16 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="18">
         <v>2363</v>
@@ -1950,28 +1964,28 @@
         <v>-1.2999999999999999E-2</v>
       </c>
       <c r="P7" s="17">
-        <v>67.5</v>
+        <v>64.8</v>
       </c>
       <c r="Q7" s="18">
-        <v>14</v>
+        <v>7.4</v>
       </c>
       <c r="R7" s="18">
-        <v>0.9</v>
+        <v>2.9</v>
       </c>
       <c r="S7" s="18">
+        <v>7.7</v>
+      </c>
+      <c r="T7" s="18">
         <v>1.6</v>
       </c>
-      <c r="T7" s="18">
+      <c r="U7" s="18">
         <v>0.1</v>
       </c>
-      <c r="U7" s="18">
-        <v>15.1</v>
-      </c>
       <c r="V7" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="W7" s="19">
-        <v>0.5</v>
+        <v>15.5</v>
+      </c>
+      <c r="W7" s="18">
+        <v>0.1</v>
       </c>
       <c r="X7" s="17">
         <v>11.4</v>
@@ -2009,16 +2023,16 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E8" s="22">
         <v>1689</v>
@@ -2054,28 +2068,28 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="P8" s="21">
-        <v>17.3</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="Q8" s="22">
-        <v>57.7</v>
+        <v>23.2</v>
       </c>
       <c r="R8" s="22">
-        <v>0.1</v>
+        <v>29.9</v>
       </c>
       <c r="S8" s="22">
+        <v>4.8</v>
+      </c>
+      <c r="T8" s="22">
         <v>0.7</v>
       </c>
-      <c r="T8" s="5">
+      <c r="U8" s="22">
         <v>21</v>
       </c>
-      <c r="U8" s="22">
-        <v>2.7</v>
-      </c>
       <c r="V8" s="22">
-        <v>0.4</v>
-      </c>
-      <c r="W8" s="23">
-        <v>0.1</v>
+        <v>3.1</v>
+      </c>
+      <c r="W8" s="5">
+        <v>0</v>
       </c>
       <c r="X8" s="21">
         <v>39.5</v>
@@ -2113,16 +2127,16 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" s="5">
         <v>3900</v>
@@ -2158,28 +2172,28 @@
         <v>-2.7E-2</v>
       </c>
       <c r="P9" s="6">
-        <v>38.9</v>
+        <v>38.6</v>
       </c>
       <c r="Q9" s="5">
-        <v>49.3</v>
+        <v>22.1</v>
       </c>
       <c r="R9" s="5">
-        <v>0.4</v>
+        <v>23</v>
       </c>
       <c r="S9" s="5">
+        <v>5.4</v>
+      </c>
+      <c r="T9" s="5">
         <v>1.5</v>
       </c>
-      <c r="T9" s="25">
+      <c r="U9" s="5">
         <v>0.5</v>
       </c>
-      <c r="U9" s="5">
-        <v>7.8</v>
-      </c>
       <c r="V9" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="W9" s="7">
-        <v>0.6</v>
+        <v>8.9</v>
+      </c>
+      <c r="W9" s="25">
+        <v>0.1</v>
       </c>
       <c r="X9" s="6">
         <v>10.5</v>
@@ -2217,16 +2231,16 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" s="5">
         <v>2592</v>
@@ -2262,28 +2276,28 @@
         <v>-2.1000000000000001E-2</v>
       </c>
       <c r="P10" s="6">
-        <v>23.3</v>
+        <v>23.2</v>
       </c>
       <c r="Q10" s="5">
-        <v>31.9</v>
+        <v>16.7</v>
       </c>
       <c r="R10" s="5">
+        <v>14.6</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="V10" s="5">
+        <v>43.5</v>
+      </c>
+      <c r="W10" s="5">
         <v>0.1</v>
-      </c>
-      <c r="S10" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="T10" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="U10" s="5">
-        <v>41.2</v>
-      </c>
-      <c r="V10" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="W10" s="7">
-        <v>0.3</v>
       </c>
       <c r="X10" s="6">
         <v>15.1</v>
@@ -2321,16 +2335,16 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5">
         <v>4036</v>
@@ -2366,26 +2380,28 @@
         <v>-1.7000000000000001E-2</v>
       </c>
       <c r="P11" s="6">
-        <v>43.5</v>
+        <v>43.3</v>
       </c>
       <c r="Q11" s="5">
-        <v>49.4</v>
+        <v>27.4</v>
       </c>
       <c r="R11" s="5">
-        <v>0.5</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="S11" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="T11" s="5">
         <v>0.7</v>
       </c>
-      <c r="T11" s="5"/>
       <c r="U11" s="5">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="V11" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="W11" s="7">
-        <v>0.3</v>
+        <v>5.7</v>
+      </c>
+      <c r="W11" s="5">
+        <v>0</v>
       </c>
       <c r="X11" s="6">
         <v>3.8</v>
@@ -2423,16 +2439,16 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="18">
         <v>538</v>
@@ -2468,26 +2484,28 @@
         <v>-0.01</v>
       </c>
       <c r="P12" s="17">
-        <v>41.1</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="18">
-        <v>48.3</v>
+        <v>29.6</v>
       </c>
       <c r="R12" s="18">
-        <v>1.7</v>
+        <v>13.2</v>
       </c>
       <c r="S12" s="18">
+        <v>10.8</v>
+      </c>
+      <c r="T12" s="18">
         <v>2.5</v>
       </c>
-      <c r="T12" s="26"/>
       <c r="U12" s="18">
+        <v>0</v>
+      </c>
+      <c r="V12" s="18">
         <v>0.4</v>
       </c>
-      <c r="V12" s="18">
-        <v>0</v>
-      </c>
-      <c r="W12" s="19">
-        <v>5.9</v>
+      <c r="W12" s="26">
+        <v>2.5</v>
       </c>
       <c r="X12" s="17">
         <v>15.4</v>
@@ -2525,16 +2543,16 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" s="5">
         <v>466</v>
@@ -2570,28 +2588,28 @@
         <v>0.03</v>
       </c>
       <c r="P13" s="6">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
       <c r="Q13" s="5">
-        <v>47</v>
+        <v>15.2</v>
       </c>
       <c r="R13" s="5">
-        <v>0.3</v>
+        <v>21.6</v>
       </c>
       <c r="S13" s="5">
+        <v>12.9</v>
+      </c>
+      <c r="T13" s="5">
         <v>0.6</v>
       </c>
-      <c r="T13" s="25">
-        <v>34.5</v>
-      </c>
       <c r="U13" s="5">
-        <v>6.7</v>
+        <v>35.1</v>
       </c>
       <c r="V13" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="W13" s="7">
-        <v>4.4000000000000004</v>
+        <v>7</v>
+      </c>
+      <c r="W13" s="25">
+        <v>1.5</v>
       </c>
       <c r="X13" s="6">
         <v>27.6</v>
@@ -2629,16 +2647,16 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="5">
         <v>1657</v>
@@ -2674,28 +2692,28 @@
         <v>-2.8000000000000001E-2</v>
       </c>
       <c r="P14" s="6">
-        <v>23.6</v>
+        <v>24.2</v>
       </c>
       <c r="Q14" s="5">
-        <v>49.1</v>
+        <v>23.9</v>
       </c>
       <c r="R14" s="5">
-        <v>1.2</v>
+        <v>21.4</v>
       </c>
       <c r="S14" s="5">
-        <v>3.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="T14" s="5">
+        <v>3.6</v>
+      </c>
+      <c r="U14" s="5">
         <v>0.9</v>
       </c>
-      <c r="U14" s="5">
-        <v>15</v>
-      </c>
       <c r="V14" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="W14" s="7">
-        <v>5.4</v>
+        <v>17.100000000000001</v>
+      </c>
+      <c r="W14" s="5">
+        <v>0.6</v>
       </c>
       <c r="X14" s="6">
         <v>13.1</v>
@@ -2733,16 +2751,16 @@
     </row>
     <row r="15" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" s="9">
         <v>3194</v>
@@ -2778,26 +2796,28 @@
         <v>-4.2000000000000003E-2</v>
       </c>
       <c r="P15" s="8">
-        <v>41.1</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="Q15" s="9">
-        <v>51.3</v>
+        <v>27.3</v>
       </c>
       <c r="R15" s="9">
-        <v>0.5</v>
+        <v>18.8</v>
       </c>
       <c r="S15" s="9">
+        <v>6.1</v>
+      </c>
+      <c r="T15" s="9">
         <v>0.7</v>
       </c>
-      <c r="T15" s="9"/>
       <c r="U15" s="9">
-        <v>5.8</v>
+        <v>0</v>
       </c>
       <c r="V15" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="W15" s="10">
-        <v>0.2</v>
+        <v>6.2</v>
+      </c>
+      <c r="W15" s="9">
+        <v>0.1</v>
       </c>
       <c r="X15" s="8">
         <v>4.9000000000000004</v>
@@ -2843,16 +2863,6 @@
         <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:W15">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -2890,11 +2900,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P2:W15">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC273F68D44EF549AD1BD0E5D55B5B7C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="315063b799ab555b4e77865ce3b3361e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="35b81125-b047-47c8-b0b0-722baac7a528" xmlns:ns3="5fe89d89-77ff-4a7d-998d-403e04f568fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cfebddd8dbdab9d9b5a54d21a7ba6ecf" ns2:_="" ns3:_="">
     <xsd:import namespace="35b81125-b047-47c8-b0b0-722baac7a528"/>
@@ -3099,15 +3128,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3115,6 +3135,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB894063-DC05-4856-80EA-85608E1C259A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC82E5DB-FE26-4367-9CC7-F53ADB13D439}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3133,14 +3161,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB894063-DC05-4856-80EA-85608E1C259A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4A86CA0-EF49-4650-8CD5-71490CFDB9D6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Exclude trips like 'walk the dog' from the survey
</commit_message>
<xml_diff>
--- a/docs/data/output/survey_processing/eda_scheme6.xlsx
+++ b/docs/data/output/survey_processing/eda_scheme6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TRM\trm_project\repo_trmg2\docs\data\output\survey_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE092756-534A-4618-8788-AEA9C7697229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E261D-358C-45E0-9F73-C6DAE99A623A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>tour_type</t>
   </si>
@@ -73,9 +73,6 @@
     <t>pct_auto_pay</t>
   </si>
   <si>
-    <t>pct_bus</t>
-  </si>
-  <si>
     <t>pct_school_bus</t>
   </si>
   <si>
@@ -164,6 +161,15 @@
   </si>
   <si>
     <t>pct_walkbike</t>
+  </si>
+  <si>
+    <t>pct_other_auto</t>
+  </si>
+  <si>
+    <t>pct_lb</t>
+  </si>
+  <si>
+    <t>pct_eb</t>
   </si>
 </sst>
 </file>
@@ -1287,15 +1293,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH15"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1345,72 +1349,78 @@
         <v>15</v>
       </c>
       <c r="Q1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="T1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="W1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="AA1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="AB1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AD1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AE1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AF1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AH1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AI1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2">
         <v>324</v>
@@ -1455,79 +1465,75 @@
         <v>48.4</v>
       </c>
       <c r="S2" s="5">
+        <v>0</v>
+      </c>
+      <c r="T2" s="5">
         <v>0.2</v>
       </c>
-      <c r="T2" s="5"/>
-      <c r="U2" s="25">
+      <c r="U2" s="5">
         <v>0</v>
       </c>
       <c r="V2" s="5">
+        <v>0</v>
+      </c>
+      <c r="W2" s="5">
+        <v>0</v>
+      </c>
+      <c r="X2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="25">
         <v>0.8</v>
       </c>
-      <c r="W2" s="25">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
+      <c r="Z2" s="1">
         <v>53.1</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="AA2" s="2">
         <v>6.2</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AB2" s="2">
         <v>26.4</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AC2" s="3">
         <v>14.3</v>
       </c>
-      <c r="AB2" s="4">
-        <v>5.39</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>-7.0000000000000001E-3</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>-3.6999999999999998E-2</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>3.1E-2</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>-3.6999999999999998E-2</v>
-      </c>
+      <c r="AD2" s="4">
+        <v>5.86</v>
+      </c>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="3"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="5">
-        <v>1873</v>
+        <v>1851</v>
       </c>
       <c r="F3" s="5">
-        <v>339400</v>
+        <v>332436</v>
       </c>
       <c r="G3" s="6">
-        <v>-8.5000000000000006E-2</v>
+        <v>-8.3000000000000004E-2</v>
       </c>
       <c r="H3" s="5">
-        <v>0.38100000000000001</v>
+        <v>0.379</v>
       </c>
       <c r="I3" s="5">
-        <v>-5.5E-2</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
       <c r="J3" s="5">
         <v>-0.14000000000000001</v>
@@ -1536,123 +1542,117 @@
         <v>-0.10100000000000001</v>
       </c>
       <c r="L3" s="5">
-        <v>-0.19</v>
+        <v>-0.189</v>
       </c>
       <c r="M3" s="5">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="N3" s="5">
-        <v>4.2000000000000003E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="O3" s="7">
-        <v>-1.6E-2</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
       <c r="P3" s="6">
-        <v>67.2</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="Q3" s="5">
-        <v>15.8</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="R3" s="5">
-        <v>10.1</v>
+        <v>10.3</v>
       </c>
       <c r="S3" s="5">
-        <v>1.8</v>
+        <v>0.1</v>
       </c>
       <c r="T3" s="5">
-        <v>0.8</v>
+        <v>1.7</v>
       </c>
       <c r="U3" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="X3" s="5">
         <v>0</v>
       </c>
-      <c r="V3" s="5">
-        <v>4.3</v>
-      </c>
-      <c r="W3" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="X3" s="6">
-        <v>15.4</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>15.1</v>
-      </c>
-      <c r="Z3" s="5">
+      <c r="Y3" s="25">
+        <v>2.7</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>15.2</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>15</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>30.1</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="AD3" s="15">
+        <v>7.29</v>
+      </c>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="7"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AA3" s="7">
-        <v>39.5</v>
-      </c>
-      <c r="AB3" s="15">
-        <v>5.47</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="AD3" s="5">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="AE3" s="5">
-        <v>9.4E-2</v>
-      </c>
-      <c r="AF3" s="5">
-        <v>1.6E-2</v>
-      </c>
-      <c r="AG3" s="5">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="AH3" s="7">
-        <v>0.112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="18">
-        <v>3566</v>
+        <v>3564</v>
       </c>
       <c r="F4" s="18">
-        <v>639632</v>
+        <v>637956</v>
       </c>
       <c r="G4" s="17">
-        <v>-0.12</v>
+        <v>-0.11899999999999999</v>
       </c>
       <c r="H4" s="18">
-        <v>0.55600000000000005</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="I4" s="18">
-        <v>-4.3999999999999997E-2</v>
+        <v>-4.2000000000000003E-2</v>
       </c>
       <c r="J4" s="18">
         <v>-0.21</v>
       </c>
       <c r="K4" s="18">
-        <v>-0.14199999999999999</v>
+        <v>-0.14099999999999999</v>
       </c>
       <c r="L4" s="18">
         <v>-0.27600000000000002</v>
       </c>
       <c r="M4" s="18">
-        <v>-4.8000000000000001E-2</v>
+        <v>-4.7E-2</v>
       </c>
       <c r="N4" s="18">
-        <v>4.4999999999999998E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="O4" s="19">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="P4" s="17">
-        <v>85.3</v>
+        <v>85.5</v>
       </c>
       <c r="Q4" s="18">
         <v>4.8</v>
@@ -1661,66 +1661,60 @@
         <v>1.8</v>
       </c>
       <c r="S4" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="T4" s="18">
+        <v>2.4</v>
+      </c>
+      <c r="U4" s="18">
+        <v>1.7</v>
+      </c>
+      <c r="V4" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="W4" s="18">
+        <v>0</v>
+      </c>
+      <c r="X4" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="26">
         <v>2.9</v>
       </c>
-      <c r="T4" s="18">
-        <v>2.1</v>
-      </c>
-      <c r="U4" s="18">
-        <v>0</v>
-      </c>
-      <c r="V4" s="18">
-        <v>3.1</v>
-      </c>
-      <c r="W4" s="26">
-        <v>0</v>
-      </c>
-      <c r="X4" s="17">
-        <v>28.8</v>
-      </c>
-      <c r="Y4" s="18">
+      <c r="Z4" s="17">
+        <v>28.9</v>
+      </c>
+      <c r="AA4" s="18">
         <v>19.3</v>
       </c>
-      <c r="Z4" s="18">
-        <v>28.2</v>
-      </c>
-      <c r="AA4" s="19">
-        <v>23.7</v>
-      </c>
-      <c r="AB4" s="20">
-        <v>10.72</v>
-      </c>
-      <c r="AC4" s="17">
-        <v>0.58599999999999997</v>
-      </c>
-      <c r="AD4" s="18">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="AE4" s="18">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="AF4" s="18">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="AG4" s="18">
-        <v>0.16</v>
-      </c>
-      <c r="AH4" s="19">
-        <v>0.39700000000000002</v>
-      </c>
+      <c r="AB4" s="18">
+        <v>28.3</v>
+      </c>
+      <c r="AC4" s="19">
+        <v>23.5</v>
+      </c>
+      <c r="AD4" s="20">
+        <v>12.01</v>
+      </c>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="19"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="22">
         <v>357</v>
@@ -1765,289 +1759,271 @@
         <v>11.1</v>
       </c>
       <c r="S5" s="22">
+        <v>0</v>
+      </c>
+      <c r="T5" s="22">
         <v>0.1</v>
       </c>
-      <c r="T5" s="22">
-        <v>0.3</v>
-      </c>
       <c r="U5" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="V5" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="W5" s="5">
         <v>0</v>
       </c>
-      <c r="V5" s="22">
+      <c r="X5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="25">
         <v>1.3</v>
       </c>
-      <c r="W5" s="25">
+      <c r="Z5" s="21">
+        <v>50.7</v>
+      </c>
+      <c r="AA5" s="22">
+        <v>14.2</v>
+      </c>
+      <c r="AB5" s="22">
+        <v>30.5</v>
+      </c>
+      <c r="AC5" s="23">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AD5" s="24">
+        <v>8.06</v>
+      </c>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22"/>
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="23"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2194</v>
+      </c>
+      <c r="F6" s="5">
+        <v>779066</v>
+      </c>
+      <c r="G6" s="6">
+        <v>-0.10199999999999999</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="I6" s="5">
+        <v>-6.9000000000000006E-2</v>
+      </c>
+      <c r="J6" s="5">
+        <v>-0.127</v>
+      </c>
+      <c r="K6" s="5">
+        <v>-9.1999999999999998E-2</v>
+      </c>
+      <c r="L6" s="5">
+        <v>-0.17699999999999999</v>
+      </c>
+      <c r="M6" s="5">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="N6" s="5">
+        <v>3.9E-2</v>
+      </c>
+      <c r="O6" s="7">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="P6" s="6">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>10.4</v>
+      </c>
+      <c r="R6" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="T6" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="U6" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="V6" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="X6" s="5">
         <v>0</v>
       </c>
-      <c r="X5" s="21">
-        <v>50.7</v>
-      </c>
-      <c r="Y5" s="22">
-        <v>14.2</v>
-      </c>
-      <c r="Z5" s="22">
-        <v>30.5</v>
-      </c>
-      <c r="AA5" s="23">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AB5" s="24">
-        <v>7.41</v>
-      </c>
-      <c r="AC5" s="21">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="AD5" s="22">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="AE5" s="22">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="AF5" s="22">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="AG5" s="22">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="AH5" s="23">
-        <v>9.5000000000000001E-2</v>
-      </c>
+      <c r="Y6" s="25">
+        <v>12.2</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>11</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>44.8</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>30.8</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>13.5</v>
+      </c>
+      <c r="AD6" s="15">
+        <v>6.25</v>
+      </c>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="7"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="5">
-        <v>743</v>
-      </c>
-      <c r="F6" s="5">
-        <v>234448</v>
-      </c>
-      <c r="G6" s="6">
-        <v>-6.6000000000000003E-2</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="I6" s="5">
-        <v>-3.7999999999999999E-2</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="D7" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="18">
+        <v>344</v>
+      </c>
+      <c r="F7" s="18">
+        <v>103926</v>
+      </c>
+      <c r="G7" s="17">
+        <v>-0.04</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="I7" s="18">
+        <v>-2.7E-2</v>
+      </c>
+      <c r="J7" s="18">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="K7" s="18">
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="L7" s="18">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="K6" s="5">
-        <v>-5.8000000000000003E-2</v>
-      </c>
-      <c r="L6" s="5">
-        <v>-0.1</v>
-      </c>
-      <c r="M6" s="5">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="N6" s="5">
-        <v>-1E-3</v>
-      </c>
-      <c r="O6" s="7">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="P6" s="6">
-        <v>56.9</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="R6" s="5">
-        <v>10</v>
-      </c>
-      <c r="S6" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="T6" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="U6" s="5">
-        <v>0</v>
-      </c>
-      <c r="V6" s="5">
-        <v>11.5</v>
-      </c>
-      <c r="W6" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="X6" s="6">
-        <v>8.5</v>
-      </c>
-      <c r="Y6" s="5">
-        <v>31.5</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>35</v>
-      </c>
-      <c r="AA6" s="7">
-        <v>25</v>
-      </c>
-      <c r="AB6" s="15">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AC6" s="6">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="AD6" s="5">
-        <v>0.42599999999999999</v>
-      </c>
-      <c r="AE6" s="5">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="AF6" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="AG6" s="5">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="AH6" s="7">
-        <v>7.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A7" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="18">
-        <v>2363</v>
-      </c>
-      <c r="F7" s="18">
-        <v>680198</v>
-      </c>
-      <c r="G7" s="17">
-        <v>-0.10299999999999999</v>
-      </c>
-      <c r="H7" s="18">
-        <v>0.376</v>
-      </c>
-      <c r="I7" s="18">
-        <v>-7.4999999999999997E-2</v>
-      </c>
-      <c r="J7" s="18">
-        <v>-0.13300000000000001</v>
-      </c>
-      <c r="K7" s="18">
-        <v>-9.8000000000000004E-2</v>
-      </c>
-      <c r="L7" s="18">
-        <v>-0.188</v>
-      </c>
       <c r="M7" s="18">
-        <v>-0.02</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="N7" s="18">
-        <v>5.3999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="O7" s="19">
-        <v>-1.2999999999999999E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="P7" s="17">
-        <v>64.8</v>
+        <v>58.1</v>
       </c>
       <c r="Q7" s="18">
-        <v>7.4</v>
+        <v>7.9</v>
       </c>
       <c r="R7" s="18">
+        <v>5.4</v>
+      </c>
+      <c r="S7" s="18">
         <v>2.9</v>
       </c>
-      <c r="S7" s="18">
-        <v>7.7</v>
-      </c>
       <c r="T7" s="18">
-        <v>1.6</v>
+        <v>12.9</v>
       </c>
       <c r="U7" s="18">
         <v>0.1</v>
       </c>
       <c r="V7" s="18">
-        <v>15.5</v>
+        <v>0.6</v>
       </c>
       <c r="W7" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="X7" s="17">
-        <v>11.4</v>
+        <v>0</v>
+      </c>
+      <c r="X7" s="18">
+        <v>0</v>
       </c>
       <c r="Y7" s="18">
-        <v>53.3</v>
-      </c>
-      <c r="Z7" s="18">
-        <v>27.5</v>
-      </c>
-      <c r="AA7" s="19">
-        <v>7.8</v>
-      </c>
-      <c r="AB7" s="20">
-        <v>6.03</v>
-      </c>
-      <c r="AC7" s="17">
-        <v>0.59399999999999997</v>
-      </c>
-      <c r="AD7" s="18">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="AE7" s="18">
-        <v>0.13</v>
-      </c>
-      <c r="AF7" s="18">
-        <v>0.35</v>
-      </c>
-      <c r="AG7" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="AH7" s="19">
-        <v>0.40400000000000003</v>
-      </c>
+        <v>12.1</v>
+      </c>
+      <c r="Z7" s="17">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AA7" s="18">
+        <v>65</v>
+      </c>
+      <c r="AB7" s="18">
+        <v>21.1</v>
+      </c>
+      <c r="AC7" s="19">
+        <v>5.8</v>
+      </c>
+      <c r="AD7" s="20">
+        <v>6.08</v>
+      </c>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
+      <c r="AJ7" s="19"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A8" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="D8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>33</v>
-      </c>
       <c r="E8" s="22">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="F8" s="22">
-        <v>624708</v>
+        <v>622069</v>
       </c>
       <c r="G8" s="21">
-        <v>0.34</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="H8" s="22">
-        <v>-0.20300000000000001</v>
+        <v>-0.20399999999999999</v>
       </c>
       <c r="I8" s="22">
-        <v>0.26300000000000001</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="J8" s="22">
         <v>-0.16500000000000001</v>
@@ -2056,7 +2032,7 @@
         <v>-0.112</v>
       </c>
       <c r="L8" s="22">
-        <v>0.40400000000000003</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="M8" s="22">
         <v>0.29399999999999998</v>
@@ -2068,304 +2044,286 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="P8" s="21">
-        <v>17.100000000000001</v>
+        <v>17.2</v>
       </c>
       <c r="Q8" s="22">
-        <v>23.2</v>
+        <v>23.1</v>
       </c>
       <c r="R8" s="22">
-        <v>29.9</v>
+        <v>30</v>
       </c>
       <c r="S8" s="22">
-        <v>4.8</v>
+        <v>0.1</v>
       </c>
       <c r="T8" s="22">
-        <v>0.7</v>
+        <v>4.7</v>
       </c>
       <c r="U8" s="22">
-        <v>21</v>
+        <v>0.6</v>
       </c>
       <c r="V8" s="22">
-        <v>3.1</v>
+        <v>0.1</v>
       </c>
       <c r="W8" s="5">
         <v>0</v>
       </c>
-      <c r="X8" s="21">
-        <v>39.5</v>
-      </c>
-      <c r="Y8" s="22">
+      <c r="X8" s="5">
+        <v>21.1</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>2.9</v>
+      </c>
+      <c r="Z8" s="21">
+        <v>39.6</v>
+      </c>
+      <c r="AA8" s="22">
         <v>25.1</v>
       </c>
-      <c r="Z8" s="22">
+      <c r="AB8" s="22">
         <v>21.5</v>
       </c>
-      <c r="AA8" s="23">
-        <v>14</v>
-      </c>
-      <c r="AB8" s="24">
-        <v>4.92</v>
-      </c>
-      <c r="AC8" s="21">
-        <v>-5.1999999999999998E-2</v>
-      </c>
-      <c r="AD8" s="22">
-        <v>-0.108</v>
-      </c>
-      <c r="AE8" s="22">
-        <v>-4.2999999999999997E-2</v>
-      </c>
-      <c r="AF8" s="22">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="AG8" s="22">
-        <v>-0.08</v>
-      </c>
-      <c r="AH8" s="23">
-        <v>-9.1999999999999998E-2</v>
-      </c>
+      <c r="AC8" s="23">
+        <v>13.8</v>
+      </c>
+      <c r="AD8" s="24">
+        <v>5.38</v>
+      </c>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="22"/>
+      <c r="AH8" s="22"/>
+      <c r="AI8" s="22"/>
+      <c r="AJ8" s="23"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="E9" s="5">
-        <v>3900</v>
+        <v>3880</v>
       </c>
       <c r="F9" s="5">
-        <v>981669</v>
+        <v>966708</v>
       </c>
       <c r="G9" s="6">
-        <v>-6.0000000000000001E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="H9" s="5">
-        <v>-0.126</v>
+        <v>-0.128</v>
       </c>
       <c r="I9" s="5">
-        <v>-1.9E-2</v>
+        <v>-0.02</v>
       </c>
       <c r="J9" s="5">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="K9" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="M9" s="5">
         <v>-1E-3</v>
       </c>
-      <c r="L9" s="5">
-        <v>1.9E-2</v>
-      </c>
-      <c r="M9" s="5">
-        <v>-3.0000000000000001E-3</v>
-      </c>
       <c r="N9" s="5">
-        <v>-1.0999999999999999E-2</v>
+        <v>-1.2E-2</v>
       </c>
       <c r="O9" s="7">
-        <v>-2.7E-2</v>
+        <v>-2.5999999999999999E-2</v>
       </c>
       <c r="P9" s="6">
-        <v>38.6</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="Q9" s="5">
-        <v>22.1</v>
+        <v>22.5</v>
       </c>
       <c r="R9" s="5">
         <v>23</v>
       </c>
       <c r="S9" s="5">
-        <v>5.4</v>
+        <v>0.4</v>
       </c>
       <c r="T9" s="5">
-        <v>1.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="U9" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="V9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="W9" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="X9" s="5">
         <v>0.5</v>
       </c>
-      <c r="V9" s="5">
-        <v>8.9</v>
-      </c>
-      <c r="W9" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="X9" s="6">
-        <v>10.5</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>30.2</v>
-      </c>
-      <c r="Z9" s="5">
-        <v>24.7</v>
-      </c>
-      <c r="AA9" s="7">
-        <v>34.6</v>
-      </c>
-      <c r="AB9" s="15">
-        <v>6.66</v>
-      </c>
-      <c r="AC9" s="6">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="AD9" s="5">
-        <v>0.105</v>
-      </c>
-      <c r="AE9" s="5">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="AF9" s="5">
-        <v>0.108</v>
-      </c>
-      <c r="AG9" s="5">
-        <v>0.36699999999999999</v>
-      </c>
-      <c r="AH9" s="7">
-        <v>0.13600000000000001</v>
-      </c>
+      <c r="Y9" s="25">
+        <v>7.3</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>10.3</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>30.5</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>24.8</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>34.4</v>
+      </c>
+      <c r="AD9" s="15">
+        <v>7.59</v>
+      </c>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="7"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2036</v>
+      </c>
+      <c r="F10" s="5">
+        <v>610862</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="J10" s="5">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K10" s="5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="L10" s="5">
+        <v>-0.04</v>
+      </c>
+      <c r="M10" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1.4E-2</v>
+      </c>
+      <c r="O10" s="7">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="P10" s="6">
+        <v>30.5</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>22.1</v>
+      </c>
+      <c r="R10" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="U10" s="5">
+        <v>1</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0</v>
+      </c>
+      <c r="W10" s="5">
+        <v>0</v>
+      </c>
+      <c r="X10" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>25.5</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="AA10" s="5">
         <v>31</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="AB10" s="5">
+        <v>27.6</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>24.8</v>
+      </c>
+      <c r="AD10" s="15">
+        <v>4.41</v>
+      </c>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="7"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="5">
-        <v>2592</v>
-      </c>
-      <c r="F10" s="5">
-        <v>818413</v>
-      </c>
-      <c r="G10" s="6">
-        <v>-1.6E-2</v>
-      </c>
-      <c r="H10" s="5">
-        <v>-3.6999999999999998E-2</v>
-      </c>
-      <c r="I10" s="5">
-        <v>-0.05</v>
-      </c>
-      <c r="J10" s="5">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="K10" s="5">
-        <v>2.4E-2</v>
-      </c>
-      <c r="L10" s="5">
-        <v>-6.2E-2</v>
-      </c>
-      <c r="M10" s="5">
-        <v>2.7E-2</v>
-      </c>
-      <c r="N10" s="5">
-        <v>2.3E-2</v>
-      </c>
-      <c r="O10" s="7">
-        <v>-2.1000000000000001E-2</v>
-      </c>
-      <c r="P10" s="6">
-        <v>23.2</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>16.7</v>
-      </c>
-      <c r="R10" s="5">
-        <v>14.6</v>
-      </c>
-      <c r="S10" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="T10" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="U10" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="V10" s="5">
-        <v>43.5</v>
-      </c>
-      <c r="W10" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="X10" s="6">
-        <v>15.1</v>
-      </c>
-      <c r="Y10" s="5">
-        <v>30.2</v>
-      </c>
-      <c r="Z10" s="5">
-        <v>27.9</v>
-      </c>
-      <c r="AA10" s="7">
-        <v>26.8</v>
-      </c>
-      <c r="AB10" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="AC10" s="6">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="AD10" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="AE10" s="5">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="AF10" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="AG10" s="5">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="AH10" s="7">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="5">
-        <v>4036</v>
+        <v>4025</v>
       </c>
       <c r="F11" s="5">
-        <v>1130729</v>
+        <v>1127444</v>
       </c>
       <c r="G11" s="6">
         <v>-0.127</v>
       </c>
       <c r="H11" s="5">
-        <v>-0.121</v>
+        <v>-0.122</v>
       </c>
       <c r="I11" s="5">
-        <v>-0.157</v>
+        <v>-0.159</v>
       </c>
       <c r="J11" s="5">
-        <v>0.17399999999999999</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="K11" s="5">
-        <v>0.13</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="L11" s="5">
         <v>-0.152</v>
@@ -2377,99 +2335,93 @@
         <v>-2.7E-2</v>
       </c>
       <c r="O11" s="7">
-        <v>-1.7000000000000001E-2</v>
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="P11" s="6">
-        <v>43.3</v>
+        <v>43.5</v>
       </c>
       <c r="Q11" s="5">
-        <v>27.4</v>
+        <v>27.6</v>
       </c>
       <c r="R11" s="5">
         <v>19.100000000000001</v>
       </c>
       <c r="S11" s="5">
-        <v>3.8</v>
+        <v>0.5</v>
       </c>
       <c r="T11" s="5">
-        <v>0.7</v>
+        <v>3.3</v>
       </c>
       <c r="U11" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="V11" s="5">
         <v>0</v>
-      </c>
-      <c r="V11" s="5">
-        <v>5.7</v>
       </c>
       <c r="W11" s="5">
         <v>0</v>
       </c>
-      <c r="X11" s="6">
+      <c r="X11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>5.3</v>
+      </c>
+      <c r="Z11" s="6">
         <v>3.8</v>
       </c>
-      <c r="Y11" s="5">
-        <v>47.3</v>
-      </c>
-      <c r="Z11" s="5">
+      <c r="AA11" s="5">
+        <v>47.4</v>
+      </c>
+      <c r="AB11" s="5">
         <v>22.9</v>
       </c>
-      <c r="AA11" s="7">
-        <v>26</v>
-      </c>
-      <c r="AB11" s="15">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="AC11" s="6">
-        <v>0.311</v>
-      </c>
-      <c r="AD11" s="5">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="AE11" s="5">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="AF11" s="5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="AG11" s="5">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="AH11" s="7">
-        <v>0.108</v>
-      </c>
+      <c r="AC11" s="7">
+        <v>25.9</v>
+      </c>
+      <c r="AD11" s="15">
+        <v>5.41</v>
+      </c>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="7"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="18">
         <v>538</v>
       </c>
       <c r="F12" s="18">
-        <v>123622</v>
+        <v>120695</v>
       </c>
       <c r="G12" s="17">
-        <v>-5.6000000000000001E-2</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="H12" s="18">
         <v>-6.6000000000000003E-2</v>
       </c>
       <c r="I12" s="18">
-        <v>-6.9000000000000006E-2</v>
+        <v>-6.8000000000000005E-2</v>
       </c>
       <c r="J12" s="18">
-        <v>0.106</v>
+        <v>0.104</v>
       </c>
       <c r="K12" s="18">
-        <v>7.1999999999999995E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L12" s="18">
         <v>-0.05</v>
@@ -2478,301 +2430,307 @@
         <v>-4.5999999999999999E-2</v>
       </c>
       <c r="N12" s="18">
-        <v>-2.3E-2</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="O12" s="19">
-        <v>-0.01</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="P12" s="17">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q12" s="18">
-        <v>29.6</v>
+        <v>30.3</v>
       </c>
       <c r="R12" s="18">
-        <v>13.2</v>
+        <v>13.5</v>
       </c>
       <c r="S12" s="18">
-        <v>10.8</v>
+        <v>2.8</v>
       </c>
       <c r="T12" s="18">
+        <v>5.9</v>
+      </c>
+      <c r="U12" s="18">
         <v>2.5</v>
       </c>
-      <c r="U12" s="18">
+      <c r="V12" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="W12" s="18">
+        <v>2.6</v>
+      </c>
+      <c r="X12" s="18">
         <v>0</v>
       </c>
-      <c r="V12" s="18">
+      <c r="Y12" s="26">
         <v>0.4</v>
       </c>
-      <c r="W12" s="26">
-        <v>2.5</v>
-      </c>
-      <c r="X12" s="17">
-        <v>15.4</v>
-      </c>
-      <c r="Y12" s="18">
-        <v>60.8</v>
-      </c>
-      <c r="Z12" s="18">
+      <c r="Z12" s="17">
+        <v>15.5</v>
+      </c>
+      <c r="AA12" s="18">
+        <v>60.7</v>
+      </c>
+      <c r="AB12" s="18">
         <v>17.3</v>
       </c>
-      <c r="AA12" s="19">
-        <v>6.4</v>
-      </c>
-      <c r="AB12" s="20">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="AC12" s="17">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="AD12" s="18">
-        <v>6.2E-2</v>
-      </c>
-      <c r="AE12" s="18">
-        <v>-4.5999999999999999E-2</v>
+      <c r="AC12" s="19">
+        <v>6.6</v>
+      </c>
+      <c r="AD12" s="20">
+        <v>9.89</v>
+      </c>
+      <c r="AE12" s="17">
+        <v>0.34699999999999998</v>
       </c>
       <c r="AF12" s="18">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AG12" s="18">
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="AH12" s="18">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="AG12" s="18">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="AH12" s="19">
-        <v>0.41199999999999998</v>
+      <c r="AI12" s="18">
+        <v>0.123</v>
+      </c>
+      <c r="AJ12" s="19">
+        <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="E13" s="5">
         <v>466</v>
       </c>
       <c r="F13" s="5">
-        <v>124235</v>
+        <v>120223</v>
       </c>
       <c r="G13" s="6">
-        <v>0.17499999999999999</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="H13" s="5">
-        <v>-0.17299999999999999</v>
+        <v>-0.17499999999999999</v>
       </c>
       <c r="I13" s="5">
-        <v>0.189</v>
+        <v>0.192</v>
       </c>
       <c r="J13" s="5">
-        <v>-8.5999999999999993E-2</v>
+        <v>-8.6999999999999994E-2</v>
       </c>
       <c r="K13" s="5">
         <v>-5.8999999999999997E-2</v>
       </c>
       <c r="L13" s="5">
-        <v>0.34499999999999997</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="M13" s="5">
-        <v>0.109</v>
+        <v>0.113</v>
       </c>
       <c r="N13" s="5">
-        <v>6.8000000000000005E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="O13" s="7">
-        <v>0.03</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="P13" s="6">
-        <v>6.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q13" s="5">
-        <v>15.2</v>
+        <v>15.7</v>
       </c>
       <c r="R13" s="5">
-        <v>21.6</v>
+        <v>22.3</v>
       </c>
       <c r="S13" s="5">
-        <v>12.9</v>
+        <v>0.3</v>
       </c>
       <c r="T13" s="5">
-        <v>0.6</v>
+        <v>11</v>
       </c>
       <c r="U13" s="5">
-        <v>35.1</v>
+        <v>0.7</v>
       </c>
       <c r="V13" s="5">
+        <v>0</v>
+      </c>
+      <c r="W13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="X13" s="5">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="Y13" s="25">
+        <v>6.9</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>27.4</v>
+      </c>
+      <c r="AA13" s="5">
+        <v>34.4</v>
+      </c>
+      <c r="AB13" s="5">
+        <v>29</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AD13" s="15">
+        <v>5.71</v>
+      </c>
+      <c r="AE13" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="AF13" s="5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AG13" s="5">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="AH13" s="5">
+        <v>0.115</v>
+      </c>
+      <c r="AI13" s="5">
+        <v>-2.8000000000000001E-2</v>
+      </c>
+      <c r="AJ13" s="7">
+        <v>-5.5E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1584</v>
+      </c>
+      <c r="F14" s="5">
+        <v>479492</v>
+      </c>
+      <c r="G14" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H14" s="5">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="I14" s="5">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="J14" s="5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K14" s="5">
+        <v>-1E-3</v>
+      </c>
+      <c r="L14" s="5">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="M14" s="5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="N14" s="5">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="O14" s="7">
+        <v>-2.7E-2</v>
+      </c>
+      <c r="P14" s="6">
+        <v>26</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>25.5</v>
+      </c>
+      <c r="R14" s="5">
+        <v>22.8</v>
+      </c>
+      <c r="S14" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="T14" s="5">
         <v>7</v>
       </c>
-      <c r="W13" s="25">
-        <v>1.5</v>
-      </c>
-      <c r="X13" s="6">
-        <v>27.6</v>
-      </c>
-      <c r="Y13" s="5">
-        <v>34.9</v>
-      </c>
-      <c r="Z13" s="5">
-        <v>28.5</v>
-      </c>
-      <c r="AA13" s="7">
-        <v>8.9</v>
-      </c>
-      <c r="AB13" s="15">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="AC13" s="6">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AD13" s="5">
-        <v>-5.1999999999999998E-2</v>
-      </c>
-      <c r="AE13" s="5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AF13" s="5">
-        <v>0.107</v>
-      </c>
-      <c r="AG13" s="5">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="AH13" s="7">
-        <v>-3.2000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="5">
-        <v>1657</v>
-      </c>
-      <c r="F14" s="5">
-        <v>510938</v>
-      </c>
-      <c r="G14" s="6">
-        <v>-7.0000000000000001E-3</v>
-      </c>
-      <c r="H14" s="5">
-        <v>-3.3000000000000002E-2</v>
-      </c>
-      <c r="I14" s="5">
-        <v>-0.04</v>
-      </c>
-      <c r="J14" s="5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="K14" s="5">
-        <v>-2E-3</v>
-      </c>
-      <c r="L14" s="5">
-        <v>-3.1E-2</v>
-      </c>
-      <c r="M14" s="5">
-        <v>2.7E-2</v>
-      </c>
-      <c r="N14" s="5">
-        <v>-1.4999999999999999E-2</v>
-      </c>
-      <c r="O14" s="7">
-        <v>-2.8000000000000001E-2</v>
-      </c>
-      <c r="P14" s="6">
-        <v>24.2</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>23.9</v>
-      </c>
-      <c r="R14" s="5">
-        <v>21.4</v>
-      </c>
-      <c r="S14" s="5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="T14" s="5">
+      <c r="U14" s="5">
         <v>3.6</v>
       </c>
-      <c r="U14" s="5">
-        <v>0.9</v>
-      </c>
       <c r="V14" s="5">
-        <v>17.100000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="W14" s="5">
         <v>0.6</v>
       </c>
-      <c r="X14" s="6">
-        <v>13.1</v>
+      <c r="X14" s="5">
+        <v>1</v>
       </c>
       <c r="Y14" s="5">
-        <v>46</v>
-      </c>
-      <c r="Z14" s="5">
-        <v>24.6</v>
-      </c>
-      <c r="AA14" s="7">
-        <v>16.2</v>
-      </c>
-      <c r="AB14" s="15">
-        <v>4.95</v>
-      </c>
-      <c r="AC14" s="6">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="AD14" s="5">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="AE14" s="5">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="AF14" s="5">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="AG14" s="5">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="AH14" s="7">
-        <v>0.19900000000000001</v>
-      </c>
+        <v>11.9</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>13.8</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>45.8</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>24.8</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>15.6</v>
+      </c>
+      <c r="AD14" s="15">
+        <v>5.6</v>
+      </c>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="7"/>
     </row>
-    <row r="15" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="9">
-        <v>3194</v>
+        <v>3169</v>
       </c>
       <c r="F15" s="9">
-        <v>1128123</v>
+        <v>1118913</v>
       </c>
       <c r="G15" s="8">
-        <v>-8.6999999999999994E-2</v>
+        <v>-8.5000000000000006E-2</v>
       </c>
       <c r="H15" s="9">
-        <v>-0.13400000000000001</v>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="I15" s="9">
         <v>-0.13</v>
@@ -2781,77 +2739,71 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="K15" s="9">
-        <v>8.4000000000000005E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="L15" s="9">
-        <v>-0.108</v>
+        <v>-0.106</v>
       </c>
       <c r="M15" s="9">
-        <v>-3.5000000000000003E-2</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="N15" s="9">
-        <v>-6.2E-2</v>
+        <v>-6.3E-2</v>
       </c>
       <c r="O15" s="10">
-        <v>-4.2000000000000003E-2</v>
+        <v>-0.04</v>
       </c>
       <c r="P15" s="8">
-        <v>40.799999999999997</v>
+        <v>41.1</v>
       </c>
       <c r="Q15" s="9">
-        <v>27.3</v>
+        <v>27.5</v>
       </c>
       <c r="R15" s="9">
-        <v>18.8</v>
+        <v>19</v>
       </c>
       <c r="S15" s="9">
-        <v>6.1</v>
+        <v>0.5</v>
       </c>
       <c r="T15" s="9">
+        <v>5.7</v>
+      </c>
+      <c r="U15" s="9">
         <v>0.7</v>
       </c>
-      <c r="U15" s="9">
+      <c r="V15" s="9">
         <v>0</v>
-      </c>
-      <c r="V15" s="9">
-        <v>6.2</v>
       </c>
       <c r="W15" s="9">
         <v>0.1</v>
       </c>
-      <c r="X15" s="8">
+      <c r="X15" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="Z15" s="8">
         <v>4.9000000000000004</v>
       </c>
-      <c r="Y15" s="9">
+      <c r="AA15" s="9">
         <v>60.1</v>
       </c>
-      <c r="Z15" s="9">
+      <c r="AB15" s="9">
         <v>18.8</v>
       </c>
-      <c r="AA15" s="10">
-        <v>16.2</v>
-      </c>
-      <c r="AB15" s="16">
-        <v>4.58</v>
-      </c>
-      <c r="AC15" s="8">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="AD15" s="9">
-        <v>0.68</v>
-      </c>
-      <c r="AE15" s="9">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="AF15" s="9">
-        <v>1.6E-2</v>
-      </c>
-      <c r="AG15" s="9">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="AH15" s="10">
-        <v>0.108</v>
-      </c>
+      <c r="AC15" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="AD15" s="16">
+        <v>4.93</v>
+      </c>
+      <c r="AE15" s="8"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:O15">
@@ -2866,7 +2818,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:AA15">
+  <conditionalFormatting sqref="Z2:AC15">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2876,7 +2828,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB15">
+  <conditionalFormatting sqref="AD2:AD15">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2888,7 +2840,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AH15">
+  <conditionalFormatting sqref="AE2:AJ15">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2900,7 +2852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:W15">
+  <conditionalFormatting sqref="P2:Y15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>